<commit_message>
modified result  from testcase
</commit_message>
<xml_diff>
--- a/QA/Selenium/Test Cases.xlsx
+++ b/QA/Selenium/Test Cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sorin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sorin\Desktop\Junior\Modul2\Json.Start\QA\Selenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC3320F-F9C4-4535-BBB8-288416ED9CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8324511-BF61-48A7-9F76-71DD79F2ACF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
   <si>
     <t>Id</t>
   </si>
@@ -139,9 +139,6 @@
   </si>
   <si>
     <t>6)Click (Sign In)</t>
-  </si>
-  <si>
-    <t>"Access denied - wrong email address or password"</t>
   </si>
   <si>
     <t xml:space="preserve">6)Customer  is logged in </t>
@@ -963,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A10:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1173,7 +1170,7 @@
         <v>12</v>
       </c>
       <c r="E18" s="50" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F18" s="49" t="s">
         <v>34</v>
@@ -1273,7 +1270,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1284,10 +1281,10 @@
         <v>37</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
added facts for creating a new account for www.auto-piesa.ro
</commit_message>
<xml_diff>
--- a/QA/Selenium/Test Cases.xlsx
+++ b/QA/Selenium/Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sorin\Desktop\Junior\Modul2\Json.Start\QA\Selenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8324511-BF61-48A7-9F76-71DD79F2ACF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD71CDA9-D06C-4B96-8F30-F2CEF87AD1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -960,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A10:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added facts + excel for piese auto
</commit_message>
<xml_diff>
--- a/QA/Selenium/Test Cases.xlsx
+++ b/QA/Selenium/Test Cases.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sorin\Desktop\Junior\Modul2\Json.Start\QA\Selenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD71CDA9-D06C-4B96-8F30-F2CEF87AD1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E88AAD3-D8FE-468C-8140-7104148E05FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Timeanddate" sheetId="1" r:id="rId1"/>
+    <sheet name="Auto-Piesa" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="152">
   <si>
     <t>Id</t>
   </si>
@@ -78,9 +79,6 @@
     <t>2) Agree with the  privacy policy</t>
   </si>
   <si>
-    <t xml:space="preserve">3) Should bring you to a page where you can choose to Create  Account or Sign In </t>
-  </si>
-  <si>
     <t>4) A new window pops up with the required information fields for a new account</t>
   </si>
   <si>
@@ -145,13 +143,641 @@
   </si>
   <si>
     <t xml:space="preserve">Email: dunca_alexandra90@gmail.com </t>
+  </si>
+  <si>
+    <t>Registration page</t>
+  </si>
+  <si>
+    <t>Reg_#1</t>
+  </si>
+  <si>
+    <t>Name:Dunca Cristina Andreea</t>
+  </si>
+  <si>
+    <t>There should be no other account registred with this name</t>
+  </si>
+  <si>
+    <t>1) Go to "https://www.auto-piesa.ro/"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2)  Click on "Contul meu" </t>
+  </si>
+  <si>
+    <t>3) Click on "Inregistrare"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">6) Check box </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Sunt de acord ca datele personale colectate în formularul de mai sus să fie folosite pentru crearea unui cont și gestionarea comenzilor (facturare, livrare, urmărirea comenzilor, garanție)"</t>
+    </r>
+  </si>
+  <si>
+    <t>7) Click on "Continuare"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3) Should bring the user to a page where he/she can choose to Create  Account or Sign In </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3) Should bring the user  to a page where he/she can choose to Create  Account or Sign In </t>
+  </si>
+  <si>
+    <t>2) Should bring the user to a page where he/she can choose to Login(autentificare) /Recover Password(recuperare parola)/ Register(inregistrare)/Quick order(comanda rapida)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3) Registration page should be displayed </t>
+  </si>
+  <si>
+    <t>4) Complete all mandatory fields with data</t>
+  </si>
+  <si>
+    <t>5)Check Box is marked</t>
+  </si>
+  <si>
+    <t>4) Mandatory fields are completed</t>
+  </si>
+  <si>
+    <t>6)Check Box is marked</t>
+  </si>
+  <si>
+    <t>As Expected</t>
+  </si>
+  <si>
+    <t>Reg_#2</t>
+  </si>
+  <si>
+    <t>The user should be on the registration page "https://www.auto-piesa.ro/cont-nou"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name:blank                                    
+Other fields valid                </t>
+  </si>
+  <si>
+    <t>2)Complete other fields with valid data and check mandatory boxex</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Reg_#3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error "Numele si prenumele trebuie sa aiba cel putin 5 caractere" should be displayed  </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The user should be on the registration page </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"https://www.auto-piesa.ro/cont-nou"</t>
+    </r>
+  </si>
+  <si>
+    <t>Reg_#4</t>
+  </si>
+  <si>
+    <t>1) Type "a" on *"Nume si Prenume" field</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5) Check Box </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Sunt de acord cu Termeni și condiții și Politica de confidențialitate"</t>
+    </r>
+  </si>
+  <si>
+    <t>1) Leave  *"Nume si Prenume" field blank</t>
+  </si>
+  <si>
+    <t>1) Leave  *" E-Mail" field blank</t>
+  </si>
+  <si>
+    <t>Reg_#5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> User should be able to complete other fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> User should  be able to complete other fields</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Email: blank                                  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Other fields valid  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Email: dunca204                                 
+Other fields valid     </t>
+  </si>
+  <si>
+    <t>1) Type "dunca204" on *"E-mail" field</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2)User should be able to complete other fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)Error message should be displayed for invalid email </t>
+  </si>
+  <si>
+    <t>Reg_#6</t>
+  </si>
+  <si>
+    <t>1) Type "dunca204@gmail" on *"E-mail" field</t>
+  </si>
+  <si>
+    <t>Reg_#7</t>
+  </si>
+  <si>
+    <t>Reg_#8</t>
+  </si>
+  <si>
+    <t>Reg_#9</t>
+  </si>
+  <si>
+    <t>Reg_#10</t>
+  </si>
+  <si>
+    <t>Reg_#11</t>
+  </si>
+  <si>
+    <t>Reg_#12</t>
+  </si>
+  <si>
+    <t>Reg_#13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email: "dunca204@gmail.com "                               
+Other fields valid     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email: "dunca204@gmail"                               
+Other fields valid     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name:"a"                                   
+Other fields valid       </t>
+  </si>
+  <si>
+    <t>1) Type "dunca204@gmail.com " on *"E-mail" field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email: "dunca205@abcdefghij.com"                               
+Other fields valid     </t>
+  </si>
+  <si>
+    <t>1) Type "dunca205@abcdefghij.com" on *"E-mail" field</t>
+  </si>
+  <si>
+    <t>No error displayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Registration request is accepted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email: "dunca205@alabalaportocala.blabla"                               
+Other fields valid     </t>
+  </si>
+  <si>
+    <t>1) Type "dunca205@alabalaportocala.blabla" on *"E-mail" field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email: "dunca205@gmail.com"                               
+Other fields valid     </t>
+  </si>
+  <si>
+    <t>1) Type "dunca205@gmail.com" on *"E-mail" field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password:""              Confirmation Password:""                           
+Other fields valid     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password:"dun"              Confirmation Password:"dun"                           
+Other fields valid     </t>
+  </si>
+  <si>
+    <t>1) Leave *"Parola"  and *"Confirmare parola" fields blank</t>
+  </si>
+  <si>
+    <t>1)Type"dun" on *"Parola" and  *"Confirmare Parola"</t>
+  </si>
+  <si>
+    <t>1)Error message should be displayed for invalid password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password:"      "              Confirmation Password:"      "                           
+Other fields valid     </t>
+  </si>
+  <si>
+    <t>1)Type"      " on *"Parola" and  *"Confirmare Parola"</t>
+  </si>
+  <si>
+    <t>Reg_#14</t>
+  </si>
+  <si>
+    <t>3) Registration request is denied.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2)User shouldbe able to complete other fields</t>
+  </si>
+  <si>
+    <t>7)Registration request should be accepted.</t>
+  </si>
+  <si>
+    <t>3)Registration request denied</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3)Registration request  denied.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Registration request accepted.</t>
+  </si>
+  <si>
+    <t>1)Type"Dunca Cristina" on *"Parola" and  *"Confirmare Parola"</t>
+  </si>
+  <si>
+    <t>Reg_#15</t>
+  </si>
+  <si>
+    <t>1)Type"Dunca Cristin" on *"Parola" and  *"Confirmare Parola"</t>
+  </si>
+  <si>
+    <t>Reg_#16</t>
+  </si>
+  <si>
+    <t>Create new account confirmation password has one different letter from password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password:"DuncaCristina"              Confirmation Password:"DuncaCristin"                           
+Other fields valid     </t>
+  </si>
+  <si>
+    <t>1)Type"DuncaCristina" on *"Parola" and "DuncaCristin" on  *"Confirmare Parola"</t>
+  </si>
+  <si>
+    <t>Reg_#17</t>
+  </si>
+  <si>
+    <t>Create new account, mandatory CheckBox "Sunt de acord cu Termeni și condiții și Politica de confidențialitate" NOT marked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other fields valid     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)Complete other fields with valid data </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1)User should be able to complete other fields</t>
+  </si>
+  <si>
+    <t>2)Check Box is marked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password:"Dunca Cristin"              Confirmation Password:"Dunca Cristin"                           Name:Dunca Cristina
+Other fields valid     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password:"Dunca Cristina"              Confirmation Password:"Dunca Cristina"                           
+Name:Dunca Cristina
+Other fields valid       </t>
+  </si>
+  <si>
+    <t>Reg_#18</t>
+  </si>
+  <si>
+    <t>Create new account, mandatory Check box "Sunt de acord ca datele personale colectate în formularul de mai sus să fie folosite pentru crearea unui cont și gestionarea comenzilor (facturare, livrare, urmărirea comenzilor, garanție)" NOT marked</t>
+  </si>
+  <si>
+    <t>2)CheckBox "Sunt de acord cu Termeni și condiții și Politica de confidențialitate"</t>
+  </si>
+  <si>
+    <t>2) Check box "Sunt de acord ca datele personale colectate în formularul de mai sus să fie folosite pentru crearea unui cont și gestionarea comenzilor (facturare, livrare, urmărirea comenzilor, garanție)"</t>
+  </si>
+  <si>
+    <r>
+      <t>Create new account</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> password has one different letter from name</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create new account </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>password is equal with full name</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Create new account</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> password is whitespace</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create new account </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>password is shorted than 6 characters</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create new account using a </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>already registred email</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create new account </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>inexistent emailprovider inexistent email domain</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create new account </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>inexistent emailprovider existent email domain</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create new account </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>valid email having extra extra whitespace at the end</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Create new account</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> valid email provider missing domain</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Create new account</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> missing email provider</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create new account </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Email Field is empty</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create new account </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>name is one letter</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Create new account</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Name Field is empty</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create new account using </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>valid data</t>
+    </r>
+  </si>
+  <si>
+    <t>Email: dunca205@gmail.com Password: dunca205 Confirmation Password: dunca205</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create new account </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>password field is empty</t>
+    </r>
+  </si>
+  <si>
+    <t>Reg_#14 *</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password:"dunca cristina"              Confirmation Password:"dunca cristina"                           
+Name:DUNCA CRISTINA
+Other fields valid       </t>
+  </si>
+  <si>
+    <t>1)Type"dunca cristina" on *"Parola" and  *"confirmare Parola"</t>
+  </si>
+  <si>
+    <t>Create new account, password and name have the same content, password is lowercase, name is uppercase</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,8 +803,54 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,8 +869,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="30">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -575,11 +1265,103 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -678,6 +1460,91 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -960,8 +1827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A10:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1018,7 +1885,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>12</v>
@@ -1027,19 +1894,19 @@
         <v>14</v>
       </c>
       <c r="F11" s="35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G11" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="21" t="s">
-        <v>23</v>
-      </c>
       <c r="I11" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J11" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -1055,16 +1922,16 @@
         <v>16</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J12" s="25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="24"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1075,13 +1942,13 @@
         <v>15</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J13" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -1092,16 +1959,16 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J14" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -1112,16 +1979,16 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="I15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J15" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1132,16 +1999,16 @@
       <c r="E16" s="37"/>
       <c r="F16" s="37"/>
       <c r="G16" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="H16" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="I16" s="26" t="s">
-        <v>28</v>
-      </c>
       <c r="J16" s="28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="34" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1158,34 +2025,34 @@
     </row>
     <row r="18" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="C18" s="51" t="s">
         <v>32</v>
-      </c>
-      <c r="C18" s="51" t="s">
-        <v>33</v>
       </c>
       <c r="D18" s="35" t="s">
         <v>12</v>
       </c>
       <c r="E18" s="50" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F18" s="49" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G18" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="H18" s="15" t="s">
-        <v>23</v>
-      </c>
       <c r="I18" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -1201,16 +2068,16 @@
         <v>16</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="9"/>
       <c r="C20" s="38"/>
@@ -1221,13 +2088,13 @@
         <v>15</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -1238,16 +2105,16 @@
       <c r="E21" s="41"/>
       <c r="F21" s="5"/>
       <c r="G21" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H21" s="13" t="s">
-        <v>36</v>
-      </c>
       <c r="I21" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -1258,16 +2125,16 @@
       <c r="E22" s="41"/>
       <c r="F22" s="5"/>
       <c r="G22" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="I22" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -1278,16 +2145,16 @@
       <c r="E23" s="42"/>
       <c r="F23" s="43"/>
       <c r="G23" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="H23" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H23" s="13" t="s">
-        <v>38</v>
-      </c>
       <c r="I23" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -1330,4 +2197,2658 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2B07E3-5E51-4B5D-BCAF-5F148637D0B8}">
+  <dimension ref="A4:I187"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="41.44140625" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="5" max="5" width="28.109375" customWidth="1"/>
+    <col min="6" max="6" width="40" customWidth="1"/>
+    <col min="7" max="7" width="35.6640625" customWidth="1"/>
+    <col min="8" max="8" width="25" customWidth="1"/>
+    <col min="9" max="9" width="23.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="67" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="52" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="56" t="s">
+        <v>145</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I10" s="60" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="59" t="s">
+        <v>146</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="58" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I11" s="60" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="60" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I13" s="60" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I14" s="60" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="51" x14ac:dyDescent="0.3">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="61" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="I15" s="60" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="37"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="H16" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="I16" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="64" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="63" t="s">
+        <v>144</v>
+      </c>
+      <c r="D17" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="65" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="66" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="20"/>
+      <c r="H17" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="G18" s="61" t="s">
+        <v>108</v>
+      </c>
+      <c r="H18" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="I18" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="37"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="H19" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I19" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="64" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="72" t="s">
+        <v>143</v>
+      </c>
+      <c r="D20" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" s="65" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="G20" s="73" t="s">
+        <v>63</v>
+      </c>
+      <c r="H20" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I20" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="H21" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I21" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G22" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="H22" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" s="66" t="s">
+        <v>69</v>
+      </c>
+      <c r="G23" s="20"/>
+      <c r="H23" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I23" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="G24" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="H24" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I24" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="G25" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="H25" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I25" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F26" s="72" t="s">
+        <v>75</v>
+      </c>
+      <c r="G26" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="H26" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I26" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H27" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I27" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="G28" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="H28" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I28" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="56" t="s">
+        <v>140</v>
+      </c>
+      <c r="D29" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F29" s="72" t="s">
+        <v>79</v>
+      </c>
+      <c r="G29" s="27"/>
+      <c r="H29" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I29" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="75"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H30" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I30" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="G31" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="H31" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I31" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="D32" s="75" t="s">
+        <v>87</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F32" s="76" t="s">
+        <v>90</v>
+      </c>
+      <c r="G32" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="H32" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I32" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H33" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I33" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="G34" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="H34" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I34" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D35" s="75" t="s">
+        <v>91</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F35" s="76" t="s">
+        <v>92</v>
+      </c>
+      <c r="G35" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="H35" s="77" t="s">
+        <v>93</v>
+      </c>
+      <c r="I35" s="77" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H36" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I36" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="G37" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="H37" s="78" t="s">
+        <v>112</v>
+      </c>
+      <c r="I37" s="77" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" s="6"/>
+      <c r="C38" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D38" s="75" t="s">
+        <v>95</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F38" s="76" t="s">
+        <v>96</v>
+      </c>
+      <c r="G38" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="H38" s="77" t="s">
+        <v>93</v>
+      </c>
+      <c r="I38" s="77" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H39" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I39" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="G40" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="H40" s="78" t="s">
+        <v>94</v>
+      </c>
+      <c r="I40" s="77" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" s="6"/>
+      <c r="C41" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D41" s="75" t="s">
+        <v>97</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F41" s="76" t="s">
+        <v>98</v>
+      </c>
+      <c r="G41" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="H41" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I41" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="G42" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H42" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I42" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="G43" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="H43" s="79" t="s">
+        <v>56</v>
+      </c>
+      <c r="I43" s="79" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D44" s="75" t="s">
+        <v>99</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G44" s="22"/>
+      <c r="H44" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I44" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H45" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I45" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="G46" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="H46" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I46" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B47" s="6"/>
+      <c r="C47" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D47" s="75" t="s">
+        <v>100</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="G47" s="74" t="s">
+        <v>103</v>
+      </c>
+      <c r="H47" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I47" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H48" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I48" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="G49" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="H49" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I49" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D50" s="75" t="s">
+        <v>104</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G50" s="74" t="s">
+        <v>103</v>
+      </c>
+      <c r="H50" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I50" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="6"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="G51" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H51" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I51" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="G52" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="H52" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I52" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B53" s="6"/>
+      <c r="C53" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D53" s="75" t="s">
+        <v>127</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G53" s="74" t="s">
+        <v>103</v>
+      </c>
+      <c r="H53" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I53" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="6"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="G54" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H54" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I54" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="G55" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="H55" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I55" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="88" t="s">
+        <v>148</v>
+      </c>
+      <c r="B56" s="60"/>
+      <c r="C56" s="61" t="s">
+        <v>151</v>
+      </c>
+      <c r="D56" s="75" t="s">
+        <v>149</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="G56" s="74" t="s">
+        <v>103</v>
+      </c>
+      <c r="H56" s="86" t="s">
+        <v>93</v>
+      </c>
+      <c r="I56" s="86" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="6"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="75"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="G57" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H57" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I57" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" s="87" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="G58" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="H58" s="78" t="s">
+        <v>94</v>
+      </c>
+      <c r="I58" s="77" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B59" s="6"/>
+      <c r="C59" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D59" s="75" t="s">
+        <v>126</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G59" s="85" t="s">
+        <v>103</v>
+      </c>
+      <c r="H59" s="86" t="s">
+        <v>93</v>
+      </c>
+      <c r="I59" s="86" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="6"/>
+      <c r="B60" s="6"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="G60" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H60" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I60" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="G61" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="H61" s="78" t="s">
+        <v>94</v>
+      </c>
+      <c r="I61" s="77" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B62" s="6"/>
+      <c r="C62" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D62" s="75" t="s">
+        <v>118</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G62" s="74" t="s">
+        <v>103</v>
+      </c>
+      <c r="H62" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I62" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="6"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="G63" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H63" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I63" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="G64" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="H64" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I64" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B65" s="6"/>
+      <c r="C65" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F65" s="80" t="s">
+        <v>123</v>
+      </c>
+      <c r="G65" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="H65" s="81" t="s">
+        <v>56</v>
+      </c>
+      <c r="I65" s="81" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="6"/>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="61" t="s">
+        <v>131</v>
+      </c>
+      <c r="G66" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="H66" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I66" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="G67" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="H67" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I67" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="82" t="s">
+        <v>128</v>
+      </c>
+      <c r="B68" s="82"/>
+      <c r="C68" s="83" t="s">
+        <v>129</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E68" s="83" t="s">
+        <v>58</v>
+      </c>
+      <c r="F68" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="G68" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="H68" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I68" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="82"/>
+      <c r="B69" s="82"/>
+      <c r="C69" s="82"/>
+      <c r="D69" s="82"/>
+      <c r="E69" s="82"/>
+      <c r="F69" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="H69" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I69" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="84"/>
+      <c r="B70" s="84"/>
+      <c r="C70" s="84"/>
+      <c r="D70" s="84"/>
+      <c r="E70" s="84"/>
+      <c r="F70" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="G70" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="H70" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I70" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A71" s="6"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="6"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72" s="6"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6"/>
+      <c r="H72" s="6"/>
+      <c r="I72" s="6"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A73" s="6"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="6"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A74" s="6"/>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="6"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75" s="6"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="6"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A76" s="6"/>
+      <c r="B76" s="6"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="6"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A77" s="6"/>
+      <c r="B77" s="6"/>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="6"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A78" s="6"/>
+      <c r="B78" s="6"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="6"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A79" s="6"/>
+      <c r="B79" s="6"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="6"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A80" s="6"/>
+      <c r="B80" s="6"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="6"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="6"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A81" s="6"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="6"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A82" s="6"/>
+      <c r="B82" s="6"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A83" s="6"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="6"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A84" s="6"/>
+      <c r="B84" s="6"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="6"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A85" s="6"/>
+      <c r="B85" s="6"/>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="6"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="6"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A86" s="6"/>
+      <c r="B86" s="6"/>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6"/>
+      <c r="I86" s="6"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A87" s="6"/>
+      <c r="B87" s="6"/>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="6"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A88" s="6"/>
+      <c r="B88" s="6"/>
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="6"/>
+      <c r="G88" s="6"/>
+      <c r="H88" s="6"/>
+      <c r="I88" s="6"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A89" s="6"/>
+      <c r="B89" s="6"/>
+      <c r="C89" s="6"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="6"/>
+      <c r="F89" s="6"/>
+      <c r="G89" s="6"/>
+      <c r="H89" s="6"/>
+      <c r="I89" s="6"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A90" s="6"/>
+      <c r="B90" s="6"/>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="6"/>
+      <c r="G90" s="6"/>
+      <c r="H90" s="6"/>
+      <c r="I90" s="6"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A91" s="6"/>
+      <c r="B91" s="6"/>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="6"/>
+      <c r="G91" s="6"/>
+      <c r="H91" s="6"/>
+      <c r="I91" s="6"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A92" s="6"/>
+      <c r="B92" s="6"/>
+      <c r="C92" s="6"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="6"/>
+      <c r="F92" s="6"/>
+      <c r="G92" s="6"/>
+      <c r="H92" s="6"/>
+      <c r="I92" s="6"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A93" s="6"/>
+      <c r="B93" s="6"/>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="6"/>
+      <c r="F93" s="6"/>
+      <c r="G93" s="6"/>
+      <c r="H93" s="6"/>
+      <c r="I93" s="6"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A94" s="6"/>
+      <c r="B94" s="6"/>
+      <c r="C94" s="6"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="6"/>
+      <c r="F94" s="6"/>
+      <c r="G94" s="6"/>
+      <c r="H94" s="6"/>
+      <c r="I94" s="6"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A95" s="6"/>
+      <c r="B95" s="6"/>
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="6"/>
+      <c r="F95" s="6"/>
+      <c r="G95" s="6"/>
+      <c r="H95" s="6"/>
+      <c r="I95" s="6"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A96" s="6"/>
+      <c r="B96" s="6"/>
+      <c r="C96" s="6"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="6"/>
+      <c r="G96" s="6"/>
+      <c r="H96" s="6"/>
+      <c r="I96" s="6"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A97" s="6"/>
+      <c r="B97" s="6"/>
+      <c r="C97" s="6"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="6"/>
+      <c r="F97" s="6"/>
+      <c r="G97" s="6"/>
+      <c r="H97" s="6"/>
+      <c r="I97" s="6"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A98" s="6"/>
+      <c r="B98" s="6"/>
+      <c r="C98" s="6"/>
+      <c r="D98" s="6"/>
+      <c r="E98" s="6"/>
+      <c r="F98" s="6"/>
+      <c r="G98" s="6"/>
+      <c r="H98" s="6"/>
+      <c r="I98" s="6"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A99" s="6"/>
+      <c r="B99" s="6"/>
+      <c r="C99" s="6"/>
+      <c r="D99" s="6"/>
+      <c r="E99" s="6"/>
+      <c r="F99" s="6"/>
+      <c r="G99" s="6"/>
+      <c r="H99" s="6"/>
+      <c r="I99" s="6"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A100" s="6"/>
+      <c r="B100" s="6"/>
+      <c r="C100" s="6"/>
+      <c r="D100" s="6"/>
+      <c r="E100" s="6"/>
+      <c r="F100" s="6"/>
+      <c r="G100" s="6"/>
+      <c r="H100" s="6"/>
+      <c r="I100" s="6"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A101" s="6"/>
+      <c r="B101" s="6"/>
+      <c r="C101" s="6"/>
+      <c r="D101" s="6"/>
+      <c r="E101" s="6"/>
+      <c r="F101" s="6"/>
+      <c r="G101" s="6"/>
+      <c r="H101" s="6"/>
+      <c r="I101" s="6"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A102" s="6"/>
+      <c r="B102" s="6"/>
+      <c r="C102" s="6"/>
+      <c r="D102" s="6"/>
+      <c r="E102" s="6"/>
+      <c r="F102" s="6"/>
+      <c r="G102" s="6"/>
+      <c r="H102" s="6"/>
+      <c r="I102" s="6"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A103" s="6"/>
+      <c r="B103" s="6"/>
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
+      <c r="E103" s="6"/>
+      <c r="F103" s="6"/>
+      <c r="G103" s="6"/>
+      <c r="H103" s="6"/>
+      <c r="I103" s="6"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A104" s="6"/>
+      <c r="B104" s="6"/>
+      <c r="C104" s="6"/>
+      <c r="D104" s="6"/>
+      <c r="E104" s="6"/>
+      <c r="F104" s="6"/>
+      <c r="G104" s="6"/>
+      <c r="H104" s="6"/>
+      <c r="I104" s="6"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A105" s="6"/>
+      <c r="B105" s="6"/>
+      <c r="C105" s="6"/>
+      <c r="D105" s="6"/>
+      <c r="E105" s="6"/>
+      <c r="F105" s="6"/>
+      <c r="G105" s="6"/>
+      <c r="H105" s="6"/>
+      <c r="I105" s="6"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A106" s="6"/>
+      <c r="B106" s="6"/>
+      <c r="C106" s="6"/>
+      <c r="D106" s="6"/>
+      <c r="E106" s="6"/>
+      <c r="F106" s="6"/>
+      <c r="G106" s="6"/>
+      <c r="H106" s="6"/>
+      <c r="I106" s="6"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A107" s="6"/>
+      <c r="B107" s="6"/>
+      <c r="C107" s="6"/>
+      <c r="D107" s="6"/>
+      <c r="E107" s="6"/>
+      <c r="F107" s="6"/>
+      <c r="G107" s="6"/>
+      <c r="H107" s="6"/>
+      <c r="I107" s="6"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A108" s="6"/>
+      <c r="B108" s="6"/>
+      <c r="C108" s="6"/>
+      <c r="D108" s="6"/>
+      <c r="E108" s="6"/>
+      <c r="F108" s="6"/>
+      <c r="G108" s="6"/>
+      <c r="H108" s="6"/>
+      <c r="I108" s="6"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A109" s="6"/>
+      <c r="B109" s="6"/>
+      <c r="C109" s="6"/>
+      <c r="D109" s="6"/>
+      <c r="E109" s="6"/>
+      <c r="F109" s="6"/>
+      <c r="G109" s="6"/>
+      <c r="H109" s="6"/>
+      <c r="I109" s="6"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A110" s="6"/>
+      <c r="B110" s="6"/>
+      <c r="C110" s="6"/>
+      <c r="D110" s="6"/>
+      <c r="E110" s="6"/>
+      <c r="F110" s="6"/>
+      <c r="G110" s="6"/>
+      <c r="H110" s="6"/>
+      <c r="I110" s="6"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A111" s="6"/>
+      <c r="B111" s="6"/>
+      <c r="C111" s="6"/>
+      <c r="D111" s="6"/>
+      <c r="E111" s="6"/>
+      <c r="F111" s="6"/>
+      <c r="G111" s="6"/>
+      <c r="H111" s="6"/>
+      <c r="I111" s="6"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A112" s="6"/>
+      <c r="B112" s="6"/>
+      <c r="C112" s="6"/>
+      <c r="D112" s="6"/>
+      <c r="E112" s="6"/>
+      <c r="F112" s="6"/>
+      <c r="G112" s="6"/>
+      <c r="H112" s="6"/>
+      <c r="I112" s="6"/>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A113" s="6"/>
+      <c r="B113" s="6"/>
+      <c r="C113" s="6"/>
+      <c r="D113" s="6"/>
+      <c r="E113" s="6"/>
+      <c r="F113" s="6"/>
+      <c r="G113" s="6"/>
+      <c r="H113" s="6"/>
+      <c r="I113" s="6"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A114" s="6"/>
+      <c r="B114" s="6"/>
+      <c r="C114" s="6"/>
+      <c r="D114" s="6"/>
+      <c r="E114" s="6"/>
+      <c r="F114" s="6"/>
+      <c r="G114" s="6"/>
+      <c r="H114" s="6"/>
+      <c r="I114" s="6"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A115" s="6"/>
+      <c r="B115" s="6"/>
+      <c r="C115" s="6"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="6"/>
+      <c r="F115" s="6"/>
+      <c r="G115" s="6"/>
+      <c r="H115" s="6"/>
+      <c r="I115" s="6"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A116" s="6"/>
+      <c r="B116" s="6"/>
+      <c r="C116" s="6"/>
+      <c r="D116" s="6"/>
+      <c r="E116" s="6"/>
+      <c r="F116" s="6"/>
+      <c r="G116" s="6"/>
+      <c r="H116" s="6"/>
+      <c r="I116" s="6"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A117" s="6"/>
+      <c r="B117" s="6"/>
+      <c r="C117" s="6"/>
+      <c r="D117" s="6"/>
+      <c r="E117" s="6"/>
+      <c r="F117" s="6"/>
+      <c r="G117" s="6"/>
+      <c r="H117" s="6"/>
+      <c r="I117" s="6"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A118" s="6"/>
+      <c r="B118" s="6"/>
+      <c r="C118" s="6"/>
+      <c r="D118" s="6"/>
+      <c r="E118" s="6"/>
+      <c r="F118" s="6"/>
+      <c r="G118" s="6"/>
+      <c r="H118" s="6"/>
+      <c r="I118" s="6"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A119" s="6"/>
+      <c r="B119" s="6"/>
+      <c r="C119" s="6"/>
+      <c r="D119" s="6"/>
+      <c r="E119" s="6"/>
+      <c r="F119" s="6"/>
+      <c r="G119" s="6"/>
+      <c r="H119" s="6"/>
+      <c r="I119" s="6"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A120" s="6"/>
+      <c r="B120" s="6"/>
+      <c r="C120" s="6"/>
+      <c r="D120" s="6"/>
+      <c r="E120" s="6"/>
+      <c r="F120" s="6"/>
+      <c r="G120" s="6"/>
+      <c r="H120" s="6"/>
+      <c r="I120" s="6"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A121" s="6"/>
+      <c r="B121" s="6"/>
+      <c r="C121" s="6"/>
+      <c r="D121" s="6"/>
+      <c r="E121" s="6"/>
+      <c r="F121" s="6"/>
+      <c r="G121" s="6"/>
+      <c r="H121" s="6"/>
+      <c r="I121" s="6"/>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A122" s="6"/>
+      <c r="B122" s="6"/>
+      <c r="C122" s="6"/>
+      <c r="D122" s="6"/>
+      <c r="E122" s="6"/>
+      <c r="F122" s="6"/>
+      <c r="G122" s="6"/>
+      <c r="H122" s="6"/>
+      <c r="I122" s="6"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A123" s="6"/>
+      <c r="B123" s="6"/>
+      <c r="C123" s="6"/>
+      <c r="D123" s="6"/>
+      <c r="E123" s="6"/>
+      <c r="F123" s="6"/>
+      <c r="G123" s="6"/>
+      <c r="H123" s="6"/>
+      <c r="I123" s="6"/>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A124" s="6"/>
+      <c r="B124" s="6"/>
+      <c r="C124" s="6"/>
+      <c r="D124" s="6"/>
+      <c r="E124" s="6"/>
+      <c r="F124" s="6"/>
+      <c r="G124" s="6"/>
+      <c r="H124" s="6"/>
+      <c r="I124" s="6"/>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A125" s="6"/>
+      <c r="B125" s="6"/>
+      <c r="C125" s="6"/>
+      <c r="D125" s="6"/>
+      <c r="E125" s="6"/>
+      <c r="F125" s="6"/>
+      <c r="G125" s="6"/>
+      <c r="H125" s="6"/>
+      <c r="I125" s="6"/>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A126" s="6"/>
+      <c r="B126" s="6"/>
+      <c r="C126" s="6"/>
+      <c r="D126" s="6"/>
+      <c r="E126" s="6"/>
+      <c r="F126" s="6"/>
+      <c r="G126" s="6"/>
+      <c r="H126" s="6"/>
+      <c r="I126" s="6"/>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A127" s="6"/>
+      <c r="B127" s="6"/>
+      <c r="C127" s="6"/>
+      <c r="D127" s="6"/>
+      <c r="E127" s="6"/>
+      <c r="F127" s="6"/>
+      <c r="G127" s="6"/>
+      <c r="H127" s="6"/>
+      <c r="I127" s="6"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A128" s="6"/>
+      <c r="B128" s="6"/>
+      <c r="C128" s="6"/>
+      <c r="D128" s="6"/>
+      <c r="E128" s="6"/>
+      <c r="F128" s="6"/>
+      <c r="G128" s="6"/>
+      <c r="H128" s="6"/>
+      <c r="I128" s="6"/>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A129" s="6"/>
+      <c r="B129" s="6"/>
+      <c r="C129" s="6"/>
+      <c r="D129" s="6"/>
+      <c r="E129" s="6"/>
+      <c r="F129" s="6"/>
+      <c r="G129" s="6"/>
+      <c r="H129" s="6"/>
+      <c r="I129" s="6"/>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A130" s="6"/>
+      <c r="B130" s="6"/>
+      <c r="C130" s="6"/>
+      <c r="D130" s="6"/>
+      <c r="E130" s="6"/>
+      <c r="F130" s="6"/>
+      <c r="G130" s="6"/>
+      <c r="H130" s="6"/>
+      <c r="I130" s="6"/>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A131" s="6"/>
+      <c r="B131" s="6"/>
+      <c r="C131" s="6"/>
+      <c r="D131" s="6"/>
+      <c r="E131" s="6"/>
+      <c r="F131" s="6"/>
+      <c r="G131" s="6"/>
+      <c r="H131" s="6"/>
+      <c r="I131" s="6"/>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A132" s="6"/>
+      <c r="B132" s="6"/>
+      <c r="C132" s="6"/>
+      <c r="D132" s="6"/>
+      <c r="E132" s="6"/>
+      <c r="F132" s="6"/>
+      <c r="G132" s="6"/>
+      <c r="H132" s="6"/>
+      <c r="I132" s="6"/>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A133" s="6"/>
+      <c r="B133" s="6"/>
+      <c r="C133" s="6"/>
+      <c r="D133" s="6"/>
+      <c r="E133" s="6"/>
+      <c r="F133" s="6"/>
+      <c r="G133" s="6"/>
+      <c r="H133" s="6"/>
+      <c r="I133" s="6"/>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A134" s="6"/>
+      <c r="B134" s="6"/>
+      <c r="C134" s="6"/>
+      <c r="D134" s="6"/>
+      <c r="E134" s="6"/>
+      <c r="F134" s="6"/>
+      <c r="G134" s="6"/>
+      <c r="H134" s="6"/>
+      <c r="I134" s="6"/>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A135" s="6"/>
+      <c r="B135" s="6"/>
+      <c r="C135" s="6"/>
+      <c r="D135" s="6"/>
+      <c r="E135" s="6"/>
+      <c r="F135" s="6"/>
+      <c r="G135" s="6"/>
+      <c r="H135" s="6"/>
+      <c r="I135" s="6"/>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A136" s="6"/>
+      <c r="B136" s="6"/>
+      <c r="C136" s="6"/>
+      <c r="D136" s="6"/>
+      <c r="E136" s="6"/>
+      <c r="F136" s="6"/>
+      <c r="G136" s="6"/>
+      <c r="H136" s="6"/>
+      <c r="I136" s="6"/>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A137" s="6"/>
+      <c r="B137" s="6"/>
+      <c r="C137" s="6"/>
+      <c r="D137" s="6"/>
+      <c r="E137" s="6"/>
+      <c r="F137" s="6"/>
+      <c r="G137" s="6"/>
+      <c r="H137" s="6"/>
+      <c r="I137" s="6"/>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A138" s="6"/>
+      <c r="B138" s="6"/>
+      <c r="C138" s="6"/>
+      <c r="D138" s="6"/>
+      <c r="E138" s="6"/>
+      <c r="F138" s="6"/>
+      <c r="G138" s="6"/>
+      <c r="H138" s="6"/>
+      <c r="I138" s="6"/>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A139" s="6"/>
+      <c r="B139" s="6"/>
+      <c r="C139" s="6"/>
+      <c r="D139" s="6"/>
+      <c r="E139" s="6"/>
+      <c r="F139" s="6"/>
+      <c r="G139" s="6"/>
+      <c r="H139" s="6"/>
+      <c r="I139" s="6"/>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A140" s="6"/>
+      <c r="B140" s="6"/>
+      <c r="C140" s="6"/>
+      <c r="D140" s="6"/>
+      <c r="E140" s="6"/>
+      <c r="F140" s="6"/>
+      <c r="G140" s="6"/>
+      <c r="H140" s="6"/>
+      <c r="I140" s="6"/>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A141" s="6"/>
+      <c r="B141" s="6"/>
+      <c r="C141" s="6"/>
+      <c r="D141" s="6"/>
+      <c r="E141" s="6"/>
+      <c r="F141" s="6"/>
+      <c r="G141" s="6"/>
+      <c r="H141" s="6"/>
+      <c r="I141" s="6"/>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A142" s="6"/>
+      <c r="B142" s="6"/>
+      <c r="C142" s="6"/>
+      <c r="D142" s="6"/>
+      <c r="E142" s="6"/>
+      <c r="F142" s="6"/>
+      <c r="G142" s="6"/>
+      <c r="H142" s="6"/>
+      <c r="I142" s="6"/>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A143" s="6"/>
+      <c r="B143" s="6"/>
+      <c r="C143" s="6"/>
+      <c r="D143" s="6"/>
+      <c r="E143" s="6"/>
+      <c r="F143" s="6"/>
+      <c r="G143" s="6"/>
+      <c r="H143" s="6"/>
+      <c r="I143" s="6"/>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A144" s="6"/>
+      <c r="B144" s="6"/>
+      <c r="C144" s="6"/>
+      <c r="D144" s="6"/>
+      <c r="E144" s="6"/>
+      <c r="F144" s="6"/>
+      <c r="G144" s="6"/>
+      <c r="H144" s="6"/>
+      <c r="I144" s="6"/>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A145" s="6"/>
+      <c r="B145" s="6"/>
+      <c r="C145" s="6"/>
+      <c r="D145" s="6"/>
+      <c r="E145" s="6"/>
+      <c r="F145" s="6"/>
+      <c r="G145" s="6"/>
+      <c r="H145" s="6"/>
+      <c r="I145" s="6"/>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A146" s="6"/>
+      <c r="B146" s="6"/>
+      <c r="C146" s="6"/>
+      <c r="D146" s="6"/>
+      <c r="E146" s="6"/>
+      <c r="F146" s="6"/>
+      <c r="G146" s="6"/>
+      <c r="H146" s="6"/>
+      <c r="I146" s="6"/>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A147" s="6"/>
+      <c r="B147" s="6"/>
+      <c r="C147" s="6"/>
+      <c r="D147" s="6"/>
+      <c r="E147" s="6"/>
+      <c r="F147" s="6"/>
+      <c r="G147" s="6"/>
+      <c r="H147" s="6"/>
+      <c r="I147" s="6"/>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A148" s="6"/>
+      <c r="B148" s="6"/>
+      <c r="C148" s="6"/>
+      <c r="D148" s="6"/>
+      <c r="E148" s="6"/>
+      <c r="F148" s="6"/>
+      <c r="G148" s="6"/>
+      <c r="H148" s="6"/>
+      <c r="I148" s="6"/>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A149" s="6"/>
+      <c r="B149" s="6"/>
+      <c r="C149" s="6"/>
+      <c r="D149" s="6"/>
+      <c r="E149" s="6"/>
+      <c r="F149" s="6"/>
+      <c r="G149" s="6"/>
+      <c r="H149" s="6"/>
+      <c r="I149" s="6"/>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A150" s="6"/>
+      <c r="B150" s="6"/>
+      <c r="C150" s="6"/>
+      <c r="D150" s="6"/>
+      <c r="E150" s="6"/>
+      <c r="F150" s="6"/>
+      <c r="G150" s="6"/>
+      <c r="H150" s="6"/>
+      <c r="I150" s="6"/>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A151" s="6"/>
+      <c r="B151" s="6"/>
+      <c r="C151" s="6"/>
+      <c r="D151" s="6"/>
+      <c r="E151" s="6"/>
+      <c r="F151" s="6"/>
+      <c r="G151" s="6"/>
+      <c r="H151" s="6"/>
+      <c r="I151" s="6"/>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A152" s="6"/>
+      <c r="B152" s="6"/>
+      <c r="C152" s="6"/>
+      <c r="D152" s="6"/>
+      <c r="E152" s="6"/>
+      <c r="F152" s="6"/>
+      <c r="G152" s="6"/>
+      <c r="H152" s="6"/>
+      <c r="I152" s="6"/>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A153" s="6"/>
+      <c r="B153" s="6"/>
+      <c r="C153" s="6"/>
+      <c r="D153" s="6"/>
+      <c r="E153" s="6"/>
+      <c r="F153" s="6"/>
+      <c r="G153" s="6"/>
+      <c r="H153" s="6"/>
+      <c r="I153" s="6"/>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A154" s="6"/>
+      <c r="B154" s="6"/>
+      <c r="C154" s="6"/>
+      <c r="D154" s="6"/>
+      <c r="E154" s="6"/>
+      <c r="F154" s="6"/>
+      <c r="G154" s="6"/>
+      <c r="H154" s="6"/>
+      <c r="I154" s="6"/>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A155" s="6"/>
+      <c r="B155" s="6"/>
+      <c r="C155" s="6"/>
+      <c r="D155" s="6"/>
+      <c r="E155" s="6"/>
+      <c r="F155" s="6"/>
+      <c r="G155" s="6"/>
+      <c r="H155" s="6"/>
+      <c r="I155" s="6"/>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A156" s="6"/>
+      <c r="B156" s="6"/>
+      <c r="C156" s="6"/>
+      <c r="D156" s="6"/>
+      <c r="E156" s="6"/>
+      <c r="F156" s="6"/>
+      <c r="G156" s="6"/>
+      <c r="H156" s="6"/>
+      <c r="I156" s="6"/>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A157" s="6"/>
+      <c r="B157" s="6"/>
+      <c r="C157" s="6"/>
+      <c r="D157" s="6"/>
+      <c r="E157" s="6"/>
+      <c r="F157" s="6"/>
+      <c r="G157" s="6"/>
+      <c r="H157" s="6"/>
+      <c r="I157" s="6"/>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A158" s="6"/>
+      <c r="B158" s="6"/>
+      <c r="C158" s="6"/>
+      <c r="D158" s="6"/>
+      <c r="E158" s="6"/>
+      <c r="F158" s="6"/>
+      <c r="G158" s="6"/>
+      <c r="H158" s="6"/>
+      <c r="I158" s="6"/>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A159" s="6"/>
+      <c r="B159" s="6"/>
+      <c r="C159" s="6"/>
+      <c r="D159" s="6"/>
+      <c r="E159" s="6"/>
+      <c r="F159" s="6"/>
+      <c r="G159" s="6"/>
+      <c r="H159" s="6"/>
+      <c r="I159" s="6"/>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A160" s="6"/>
+      <c r="B160" s="6"/>
+      <c r="C160" s="6"/>
+      <c r="D160" s="6"/>
+      <c r="E160" s="6"/>
+      <c r="F160" s="6"/>
+      <c r="G160" s="6"/>
+      <c r="H160" s="6"/>
+      <c r="I160" s="6"/>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A161" s="6"/>
+      <c r="B161" s="6"/>
+      <c r="C161" s="6"/>
+      <c r="D161" s="6"/>
+      <c r="E161" s="6"/>
+      <c r="F161" s="6"/>
+      <c r="G161" s="6"/>
+      <c r="H161" s="6"/>
+      <c r="I161" s="6"/>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A162" s="6"/>
+      <c r="B162" s="6"/>
+      <c r="C162" s="6"/>
+      <c r="D162" s="6"/>
+      <c r="E162" s="6"/>
+      <c r="F162" s="6"/>
+      <c r="G162" s="6"/>
+      <c r="H162" s="6"/>
+      <c r="I162" s="6"/>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A163" s="6"/>
+      <c r="B163" s="6"/>
+      <c r="C163" s="6"/>
+      <c r="D163" s="6"/>
+      <c r="E163" s="6"/>
+      <c r="F163" s="6"/>
+      <c r="G163" s="6"/>
+      <c r="H163" s="6"/>
+      <c r="I163" s="6"/>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A164" s="6"/>
+      <c r="B164" s="6"/>
+      <c r="C164" s="6"/>
+      <c r="D164" s="6"/>
+      <c r="E164" s="6"/>
+      <c r="F164" s="6"/>
+      <c r="G164" s="6"/>
+      <c r="H164" s="6"/>
+      <c r="I164" s="6"/>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A165" s="6"/>
+      <c r="B165" s="6"/>
+      <c r="C165" s="6"/>
+      <c r="D165" s="6"/>
+      <c r="E165" s="6"/>
+      <c r="F165" s="6"/>
+      <c r="G165" s="6"/>
+      <c r="H165" s="6"/>
+      <c r="I165" s="6"/>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A166" s="6"/>
+      <c r="B166" s="6"/>
+      <c r="C166" s="6"/>
+      <c r="D166" s="6"/>
+      <c r="E166" s="6"/>
+      <c r="F166" s="6"/>
+      <c r="G166" s="6"/>
+      <c r="H166" s="6"/>
+      <c r="I166" s="6"/>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A167" s="6"/>
+      <c r="B167" s="6"/>
+      <c r="C167" s="6"/>
+      <c r="D167" s="6"/>
+      <c r="E167" s="6"/>
+      <c r="F167" s="6"/>
+      <c r="G167" s="6"/>
+      <c r="H167" s="6"/>
+      <c r="I167" s="6"/>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A168" s="6"/>
+      <c r="B168" s="6"/>
+      <c r="C168" s="6"/>
+      <c r="D168" s="6"/>
+      <c r="E168" s="6"/>
+      <c r="F168" s="6"/>
+      <c r="G168" s="6"/>
+      <c r="H168" s="6"/>
+      <c r="I168" s="6"/>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A169" s="6"/>
+      <c r="B169" s="6"/>
+      <c r="C169" s="6"/>
+      <c r="D169" s="6"/>
+      <c r="E169" s="6"/>
+      <c r="F169" s="6"/>
+      <c r="G169" s="6"/>
+      <c r="H169" s="6"/>
+      <c r="I169" s="6"/>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A170" s="6"/>
+      <c r="B170" s="6"/>
+      <c r="C170" s="6"/>
+      <c r="D170" s="6"/>
+      <c r="E170" s="6"/>
+      <c r="F170" s="6"/>
+      <c r="G170" s="6"/>
+      <c r="H170" s="6"/>
+      <c r="I170" s="6"/>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A171" s="6"/>
+      <c r="B171" s="6"/>
+      <c r="C171" s="6"/>
+      <c r="D171" s="6"/>
+      <c r="E171" s="6"/>
+      <c r="F171" s="6"/>
+      <c r="G171" s="6"/>
+      <c r="H171" s="6"/>
+      <c r="I171" s="6"/>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A172" s="6"/>
+      <c r="B172" s="6"/>
+      <c r="C172" s="6"/>
+      <c r="D172" s="6"/>
+      <c r="E172" s="6"/>
+      <c r="F172" s="6"/>
+      <c r="G172" s="6"/>
+      <c r="H172" s="6"/>
+      <c r="I172" s="6"/>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A173" s="6"/>
+      <c r="B173" s="6"/>
+      <c r="C173" s="6"/>
+      <c r="D173" s="6"/>
+      <c r="E173" s="6"/>
+      <c r="F173" s="6"/>
+      <c r="G173" s="6"/>
+      <c r="H173" s="6"/>
+      <c r="I173" s="6"/>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A174" s="6"/>
+      <c r="B174" s="6"/>
+      <c r="C174" s="6"/>
+      <c r="D174" s="6"/>
+      <c r="E174" s="6"/>
+      <c r="F174" s="6"/>
+      <c r="G174" s="6"/>
+      <c r="H174" s="6"/>
+      <c r="I174" s="6"/>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A175" s="6"/>
+      <c r="B175" s="6"/>
+      <c r="C175" s="6"/>
+      <c r="D175" s="6"/>
+      <c r="E175" s="6"/>
+      <c r="F175" s="6"/>
+      <c r="G175" s="6"/>
+      <c r="H175" s="6"/>
+      <c r="I175" s="6"/>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A176" s="6"/>
+      <c r="B176" s="6"/>
+      <c r="C176" s="6"/>
+      <c r="D176" s="6"/>
+      <c r="E176" s="6"/>
+      <c r="F176" s="6"/>
+      <c r="G176" s="6"/>
+      <c r="H176" s="6"/>
+      <c r="I176" s="6"/>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A177" s="6"/>
+      <c r="B177" s="6"/>
+      <c r="C177" s="6"/>
+      <c r="D177" s="6"/>
+      <c r="E177" s="6"/>
+      <c r="F177" s="6"/>
+      <c r="G177" s="6"/>
+      <c r="H177" s="6"/>
+      <c r="I177" s="6"/>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A178" s="6"/>
+      <c r="B178" s="6"/>
+      <c r="C178" s="6"/>
+      <c r="D178" s="6"/>
+      <c r="E178" s="6"/>
+      <c r="F178" s="6"/>
+      <c r="G178" s="6"/>
+      <c r="H178" s="6"/>
+      <c r="I178" s="6"/>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A179" s="6"/>
+      <c r="B179" s="6"/>
+      <c r="C179" s="6"/>
+      <c r="D179" s="6"/>
+      <c r="E179" s="6"/>
+      <c r="F179" s="6"/>
+      <c r="G179" s="6"/>
+      <c r="H179" s="6"/>
+      <c r="I179" s="6"/>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A180" s="6"/>
+      <c r="B180" s="6"/>
+      <c r="C180" s="6"/>
+      <c r="D180" s="6"/>
+      <c r="E180" s="6"/>
+      <c r="F180" s="6"/>
+      <c r="G180" s="6"/>
+      <c r="H180" s="6"/>
+      <c r="I180" s="6"/>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A181" s="6"/>
+      <c r="B181" s="6"/>
+      <c r="C181" s="6"/>
+      <c r="D181" s="6"/>
+      <c r="E181" s="6"/>
+      <c r="F181" s="6"/>
+      <c r="G181" s="6"/>
+      <c r="H181" s="6"/>
+      <c r="I181" s="6"/>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A182" s="6"/>
+      <c r="B182" s="6"/>
+      <c r="C182" s="6"/>
+      <c r="D182" s="6"/>
+      <c r="E182" s="6"/>
+      <c r="F182" s="6"/>
+      <c r="G182" s="6"/>
+      <c r="H182" s="6"/>
+      <c r="I182" s="6"/>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A183" s="6"/>
+      <c r="B183" s="6"/>
+      <c r="C183" s="6"/>
+      <c r="D183" s="6"/>
+      <c r="E183" s="6"/>
+      <c r="F183" s="6"/>
+      <c r="G183" s="6"/>
+      <c r="H183" s="6"/>
+      <c r="I183" s="6"/>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A184" s="6"/>
+      <c r="B184" s="6"/>
+      <c r="C184" s="6"/>
+      <c r="D184" s="6"/>
+      <c r="E184" s="6"/>
+      <c r="F184" s="6"/>
+      <c r="G184" s="6"/>
+      <c r="H184" s="6"/>
+      <c r="I184" s="6"/>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A185" s="6"/>
+      <c r="B185" s="6"/>
+      <c r="C185" s="6"/>
+      <c r="D185" s="6"/>
+      <c r="E185" s="6"/>
+      <c r="F185" s="6"/>
+      <c r="G185" s="6"/>
+      <c r="H185" s="6"/>
+      <c r="I185" s="6"/>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A186" s="6"/>
+      <c r="B186" s="6"/>
+      <c r="C186" s="6"/>
+      <c r="D186" s="6"/>
+      <c r="E186" s="6"/>
+      <c r="F186" s="6"/>
+      <c r="G186" s="6"/>
+      <c r="H186" s="6"/>
+      <c r="I186" s="6"/>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A187" s="6"/>
+      <c r="B187" s="6"/>
+      <c r="C187" s="6"/>
+      <c r="D187" s="6"/>
+      <c r="E187" s="6"/>
+      <c r="F187" s="6"/>
+      <c r="G187" s="6"/>
+      <c r="H187" s="6"/>
+      <c r="I187" s="6"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fact 8, 9 14 ,15 => bugs
</commit_message>
<xml_diff>
--- a/QA/Selenium/Test Cases.xlsx
+++ b/QA/Selenium/Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sorin\Desktop\Junior\Modul2\Json.Start\QA\Selenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E88AAD3-D8FE-468C-8140-7104148E05FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6D125C-C29E-4722-9CA4-1E033CBB4BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -850,7 +850,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -878,12 +878,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1361,7 +1355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1529,7 +1523,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2203,8 +2196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2B07E3-5E51-4B5D-BCAF-5F148637D0B8}">
   <dimension ref="A4:I187"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42:I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2969,10 +2962,10 @@
       <c r="G43" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="H43" s="79" t="s">
-        <v>56</v>
-      </c>
-      <c r="I43" s="79" t="s">
+      <c r="H43" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I43" s="70" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3235,7 +3228,7 @@
       </c>
     </row>
     <row r="56" spans="1:9" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="88" t="s">
+      <c r="A56" s="87" t="s">
         <v>148</v>
       </c>
       <c r="B56" s="60"/>
@@ -3254,10 +3247,10 @@
       <c r="G56" s="74" t="s">
         <v>103</v>
       </c>
-      <c r="H56" s="86" t="s">
+      <c r="H56" s="85" t="s">
         <v>93</v>
       </c>
-      <c r="I56" s="86" t="s">
+      <c r="I56" s="85" t="s">
         <v>61</v>
       </c>
     </row>
@@ -3280,7 +3273,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:9" s="87" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" s="86" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -3316,13 +3309,13 @@
       <c r="F59" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="G59" s="85" t="s">
+      <c r="G59" s="84" t="s">
         <v>103</v>
       </c>
-      <c r="H59" s="86" t="s">
+      <c r="H59" s="85" t="s">
         <v>93</v>
       </c>
-      <c r="I59" s="86" t="s">
+      <c r="I59" s="85" t="s">
         <v>61</v>
       </c>
     </row>
@@ -3443,16 +3436,16 @@
       <c r="E65" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F65" s="80" t="s">
+      <c r="F65" s="79" t="s">
         <v>123</v>
       </c>
       <c r="G65" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="H65" s="81" t="s">
-        <v>56</v>
-      </c>
-      <c r="I65" s="81" t="s">
+      <c r="H65" s="80" t="s">
+        <v>56</v>
+      </c>
+      <c r="I65" s="80" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3495,17 +3488,17 @@
       </c>
     </row>
     <row r="68" spans="1:9" ht="87" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="82" t="s">
+      <c r="A68" s="81" t="s">
         <v>128</v>
       </c>
-      <c r="B68" s="82"/>
-      <c r="C68" s="83" t="s">
+      <c r="B68" s="81"/>
+      <c r="C68" s="82" t="s">
         <v>129</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="E68" s="83" t="s">
+      <c r="E68" s="82" t="s">
         <v>58</v>
       </c>
       <c r="F68" s="20" t="s">
@@ -3522,11 +3515,11 @@
       </c>
     </row>
     <row r="69" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="82"/>
-      <c r="B69" s="82"/>
-      <c r="C69" s="82"/>
-      <c r="D69" s="82"/>
-      <c r="E69" s="82"/>
+      <c r="A69" s="81"/>
+      <c r="B69" s="81"/>
+      <c r="C69" s="81"/>
+      <c r="D69" s="81"/>
+      <c r="E69" s="81"/>
       <c r="F69" s="11" t="s">
         <v>130</v>
       </c>
@@ -3541,11 +3534,11 @@
       </c>
     </row>
     <row r="70" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="84"/>
-      <c r="B70" s="84"/>
-      <c r="C70" s="84"/>
-      <c r="D70" s="84"/>
-      <c r="E70" s="84"/>
+      <c r="A70" s="83"/>
+      <c r="B70" s="83"/>
+      <c r="C70" s="83"/>
+      <c r="D70" s="83"/>
+      <c r="E70" s="83"/>
       <c r="F70" s="69" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
added one more fact=> very long email adress
</commit_message>
<xml_diff>
--- a/QA/Selenium/Test Cases.xlsx
+++ b/QA/Selenium/Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sorin\Desktop\Junior\Modul2\Json.Start\QA\Selenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6D125C-C29E-4722-9CA4-1E033CBB4BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234D87C8-9D7E-407F-8DC5-C7D51C2AAEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="157">
   <si>
     <t>Id</t>
   </si>
@@ -771,6 +771,21 @@
   </si>
   <si>
     <t>Create new account, password and name have the same content, password is lowercase, name is uppercase</t>
+  </si>
+  <si>
+    <t>Reg_#9*</t>
+  </si>
+  <si>
+    <t>Create new account email length is larger than 1000 letters</t>
+  </si>
+  <si>
+    <t>Email: duncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristina@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Type  a word larger than 1000 letters and add "@gmail.com" on *"E-mail" field                                                                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2)Complete other fields with valid data and check mandatory boxex   </t>
   </si>
 </sst>
 </file>
@@ -1355,7 +1370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1538,6 +1553,26 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2194,10 +2229,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2B07E3-5E51-4B5D-BCAF-5F148637D0B8}">
-  <dimension ref="A4:I187"/>
+  <dimension ref="A4:I190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42:I43"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2660,7 +2695,7 @@
       <c r="E29" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F29" s="72" t="s">
+      <c r="F29" s="76" t="s">
         <v>79</v>
       </c>
       <c r="G29" s="27"/>
@@ -2905,89 +2940,87 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B41" s="6"/>
-      <c r="C41" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="D41" s="75" t="s">
-        <v>97</v>
-      </c>
-      <c r="E41" s="7" t="s">
+      <c r="A41" s="90" t="s">
+        <v>152</v>
+      </c>
+      <c r="B41" s="91"/>
+      <c r="C41" s="92" t="s">
+        <v>153</v>
+      </c>
+      <c r="D41" s="93" t="s">
+        <v>154</v>
+      </c>
+      <c r="E41" s="92" t="s">
         <v>58</v>
       </c>
-      <c r="F41" s="76" t="s">
-        <v>98</v>
+      <c r="F41" s="73" t="s">
+        <v>155</v>
       </c>
       <c r="G41" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="H41" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I41" s="70" t="s">
-        <v>28</v>
+      <c r="H41" s="77" t="s">
+        <v>93</v>
+      </c>
+      <c r="I41" s="77" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="68" t="s">
-        <v>60</v>
+      <c r="A42" s="64"/>
+      <c r="B42" s="88"/>
+      <c r="C42" s="59"/>
+      <c r="D42" s="89"/>
+      <c r="E42" s="59"/>
+      <c r="F42" s="76" t="s">
+        <v>156</v>
       </c>
       <c r="G42" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="H42" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I42" s="70" t="s">
-        <v>28</v>
-      </c>
+      <c r="H42" s="69"/>
+      <c r="I42" s="70"/>
     </row>
     <row r="43" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
+      <c r="A43" s="94"/>
+      <c r="B43" s="95"/>
+      <c r="C43" s="96"/>
+      <c r="D43" s="97"/>
+      <c r="E43" s="96"/>
       <c r="F43" s="69" t="s">
         <v>45</v>
       </c>
       <c r="G43" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="H43" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I43" s="70" t="s">
-        <v>28</v>
+      <c r="H43" s="77" t="s">
+        <v>93</v>
+      </c>
+      <c r="I43" s="77" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B44" s="6"/>
-      <c r="C44" s="6" t="s">
-        <v>147</v>
+      <c r="C44" s="7" t="s">
+        <v>136</v>
       </c>
       <c r="D44" s="75" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F44" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="G44" s="22"/>
-      <c r="H44" s="70" t="s">
+      <c r="F44" s="76" t="s">
+        <v>98</v>
+      </c>
+      <c r="G44" s="84" t="s">
+        <v>77</v>
+      </c>
+      <c r="H44" s="80" t="s">
         <v>56</v>
       </c>
       <c r="I44" s="70" t="s">
@@ -3034,24 +3067,22 @@
     </row>
     <row r="47" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B47" s="6"/>
-      <c r="C47" s="7" t="s">
-        <v>135</v>
+      <c r="C47" s="6" t="s">
+        <v>147</v>
       </c>
       <c r="D47" s="75" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>58</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="G47" s="74" t="s">
-        <v>103</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="G47" s="22"/>
       <c r="H47" s="70" t="s">
         <v>56</v>
       </c>
@@ -3099,20 +3130,20 @@
     </row>
     <row r="50" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B50" s="6"/>
-      <c r="C50" s="6" t="s">
-        <v>134</v>
+      <c r="C50" s="7" t="s">
+        <v>135</v>
       </c>
       <c r="D50" s="75" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E50" s="7" t="s">
         <v>58</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G50" s="74" t="s">
         <v>103</v>
@@ -3162,22 +3193,22 @@
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="6" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="B53" s="6"/>
-      <c r="C53" s="7" t="s">
-        <v>133</v>
+      <c r="C53" s="6" t="s">
+        <v>134</v>
       </c>
       <c r="D53" s="75" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="E53" s="7" t="s">
         <v>58</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="G53" s="74" t="s">
         <v>103</v>
@@ -3228,38 +3259,38 @@
       </c>
     </row>
     <row r="56" spans="1:9" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="87" t="s">
-        <v>148</v>
-      </c>
-      <c r="B56" s="60"/>
-      <c r="C56" s="61" t="s">
-        <v>151</v>
+      <c r="A56" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B56" s="6"/>
+      <c r="C56" s="7" t="s">
+        <v>133</v>
       </c>
       <c r="D56" s="75" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="E56" s="7" t="s">
         <v>58</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>150</v>
+        <v>113</v>
       </c>
       <c r="G56" s="74" t="s">
         <v>103</v>
       </c>
-      <c r="H56" s="85" t="s">
-        <v>93</v>
-      </c>
-      <c r="I56" s="85" t="s">
-        <v>61</v>
+      <c r="H56" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I56" s="70" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
-      <c r="C57" s="7"/>
-      <c r="D57" s="75"/>
-      <c r="E57" s="7"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
       <c r="F57" s="68" t="s">
         <v>60</v>
       </c>
@@ -3273,7 +3304,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:9" s="86" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -3285,31 +3316,31 @@
       <c r="G58" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="H58" s="78" t="s">
-        <v>94</v>
-      </c>
-      <c r="I58" s="77" t="s">
-        <v>61</v>
+      <c r="H58" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I58" s="70" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="B59" s="6"/>
-      <c r="C59" s="7" t="s">
-        <v>132</v>
+      <c r="A59" s="87" t="s">
+        <v>148</v>
+      </c>
+      <c r="B59" s="60"/>
+      <c r="C59" s="61" t="s">
+        <v>151</v>
       </c>
       <c r="D59" s="75" t="s">
-        <v>126</v>
+        <v>149</v>
       </c>
       <c r="E59" s="7" t="s">
         <v>58</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="G59" s="84" t="s">
+        <v>150</v>
+      </c>
+      <c r="G59" s="74" t="s">
         <v>103</v>
       </c>
       <c r="H59" s="85" t="s">
@@ -3322,9 +3353,9 @@
     <row r="60" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
-      <c r="C60" s="6"/>
-      <c r="D60" s="6"/>
-      <c r="E60" s="6"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="75"/>
+      <c r="E60" s="7"/>
       <c r="F60" s="68" t="s">
         <v>60</v>
       </c>
@@ -3338,7 +3369,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" s="86" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -3357,31 +3388,31 @@
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B62" s="6"/>
       <c r="C62" s="7" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
       <c r="D62" s="75" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="E62" s="7" t="s">
         <v>58</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="G62" s="74" t="s">
+        <v>115</v>
+      </c>
+      <c r="G62" s="84" t="s">
         <v>103</v>
       </c>
-      <c r="H62" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I62" s="70" t="s">
-        <v>28</v>
+      <c r="H62" s="85" t="s">
+        <v>93</v>
+      </c>
+      <c r="I62" s="85" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -3403,7 +3434,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -3415,51 +3446,51 @@
       <c r="G64" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="H64" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I64" s="70" t="s">
-        <v>28</v>
+      <c r="H64" s="78" t="s">
+        <v>94</v>
+      </c>
+      <c r="I64" s="77" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="6" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B65" s="6"/>
       <c r="C65" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>122</v>
+        <v>117</v>
+      </c>
+      <c r="D65" s="75" t="s">
+        <v>118</v>
       </c>
       <c r="E65" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F65" s="79" t="s">
-        <v>123</v>
-      </c>
-      <c r="G65" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="H65" s="80" t="s">
-        <v>56</v>
-      </c>
-      <c r="I65" s="80" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F65" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G65" s="74" t="s">
+        <v>103</v>
+      </c>
+      <c r="H65" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I65" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="6"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
       <c r="D66" s="6"/>
       <c r="E66" s="6"/>
-      <c r="F66" s="61" t="s">
-        <v>131</v>
-      </c>
-      <c r="G66" s="4" t="s">
-        <v>125</v>
+      <c r="F66" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="G66" s="12" t="s">
+        <v>76</v>
       </c>
       <c r="H66" s="70" t="s">
         <v>56</v>
@@ -3487,41 +3518,41 @@
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="87" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="81" t="s">
-        <v>128</v>
-      </c>
-      <c r="B68" s="81"/>
-      <c r="C68" s="82" t="s">
-        <v>129</v>
+    <row r="68" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B68" s="6"/>
+      <c r="C68" s="7" t="s">
+        <v>121</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="E68" s="82" t="s">
+      <c r="E68" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F68" s="20" t="s">
+      <c r="F68" s="79" t="s">
         <v>123</v>
       </c>
       <c r="G68" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="H68" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I68" s="70" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="81"/>
-      <c r="B69" s="81"/>
-      <c r="C69" s="81"/>
-      <c r="D69" s="81"/>
-      <c r="E69" s="81"/>
-      <c r="F69" s="11" t="s">
-        <v>130</v>
+      <c r="H68" s="80" t="s">
+        <v>56</v>
+      </c>
+      <c r="I68" s="80" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="6"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="61" t="s">
+        <v>131</v>
       </c>
       <c r="G69" s="4" t="s">
         <v>125</v>
@@ -3534,11 +3565,11 @@
       </c>
     </row>
     <row r="70" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="83"/>
-      <c r="B70" s="83"/>
-      <c r="C70" s="83"/>
-      <c r="D70" s="83"/>
-      <c r="E70" s="83"/>
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
       <c r="F70" s="69" t="s">
         <v>45</v>
       </c>
@@ -3552,38 +3583,70 @@
         <v>28</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A71" s="6"/>
-      <c r="B71" s="6"/>
-      <c r="C71" s="6"/>
-      <c r="D71" s="6"/>
-      <c r="E71" s="6"/>
-      <c r="F71" s="6"/>
-      <c r="G71" s="6"/>
-      <c r="H71" s="6"/>
-      <c r="I71" s="6"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72" s="6"/>
-      <c r="B72" s="6"/>
-      <c r="C72" s="6"/>
-      <c r="D72" s="6"/>
-      <c r="E72" s="6"/>
-      <c r="F72" s="6"/>
-      <c r="G72" s="6"/>
-      <c r="H72" s="6"/>
-      <c r="I72" s="6"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A73" s="6"/>
-      <c r="B73" s="6"/>
-      <c r="C73" s="6"/>
-      <c r="D73" s="6"/>
-      <c r="E73" s="6"/>
-      <c r="F73" s="6"/>
-      <c r="G73" s="6"/>
-      <c r="H73" s="6"/>
-      <c r="I73" s="6"/>
+    <row r="71" spans="1:9" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="81" t="s">
+        <v>128</v>
+      </c>
+      <c r="B71" s="81"/>
+      <c r="C71" s="82" t="s">
+        <v>129</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E71" s="82" t="s">
+        <v>58</v>
+      </c>
+      <c r="F71" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="G71" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="H71" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I71" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="81"/>
+      <c r="B72" s="81"/>
+      <c r="C72" s="81"/>
+      <c r="D72" s="81"/>
+      <c r="E72" s="81"/>
+      <c r="F72" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="H72" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I72" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="83"/>
+      <c r="B73" s="83"/>
+      <c r="C73" s="83"/>
+      <c r="D73" s="83"/>
+      <c r="E73" s="83"/>
+      <c r="F73" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="G73" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="H73" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I73" s="70" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="6"/>
@@ -4839,6 +4902,39 @@
       <c r="H187" s="6"/>
       <c r="I187" s="6"/>
     </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A188" s="6"/>
+      <c r="B188" s="6"/>
+      <c r="C188" s="6"/>
+      <c r="D188" s="6"/>
+      <c r="E188" s="6"/>
+      <c r="F188" s="6"/>
+      <c r="G188" s="6"/>
+      <c r="H188" s="6"/>
+      <c r="I188" s="6"/>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A189" s="6"/>
+      <c r="B189" s="6"/>
+      <c r="C189" s="6"/>
+      <c r="D189" s="6"/>
+      <c r="E189" s="6"/>
+      <c r="F189" s="6"/>
+      <c r="G189" s="6"/>
+      <c r="H189" s="6"/>
+      <c r="I189" s="6"/>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A190" s="6"/>
+      <c r="B190" s="6"/>
+      <c r="C190" s="6"/>
+      <c r="D190" s="6"/>
+      <c r="E190" s="6"/>
+      <c r="F190" s="6"/>
+      <c r="G190" s="6"/>
+      <c r="H190" s="6"/>
+      <c r="I190" s="6"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added facts for symbols and very long sequence of characters  (~1000 characters) for email, and name fields
</commit_message>
<xml_diff>
--- a/QA/Selenium/Test Cases.xlsx
+++ b/QA/Selenium/Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sorin\Desktop\Junior\Modul2\Json.Start\QA\Selenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFEBB2B-43DC-4401-BDA2-6AFC55E579B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384F2229-D975-45A7-BC31-70FCFA4A5D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="175">
   <si>
     <t>Id</t>
   </si>
@@ -281,9 +281,6 @@
     <t>Reg_#5</t>
   </si>
   <si>
-    <t xml:space="preserve"> User should be able to complete other fields</t>
-  </si>
-  <si>
     <t xml:space="preserve"> User should  be able to complete other fields</t>
   </si>
   <si>
@@ -452,9 +449,6 @@
     <t>Reg_#16</t>
   </si>
   <si>
-    <t>Create new account confirmation password has one different letter from password</t>
-  </si>
-  <si>
     <t xml:space="preserve">Password:"DuncaCristina"              Confirmation Password:"DuncaCristin"                           
 Other fields valid     </t>
   </si>
@@ -463,9 +457,6 @@
   </si>
   <si>
     <t>Reg_#17</t>
-  </si>
-  <si>
-    <t>Create new account, mandatory CheckBox "Sunt de acord cu Termeni și condiții și Politica de confidențialitate" NOT marked</t>
   </si>
   <si>
     <t xml:space="preserve">Other fields valid     </t>
@@ -490,9 +481,6 @@
   </si>
   <si>
     <t>Reg_#18</t>
-  </si>
-  <si>
-    <t>Create new account, mandatory Check box "Sunt de acord ca datele personale colectate în formularul de mai sus să fie folosite pentru crearea unui cont și gestionarea comenzilor (facturare, livrare, urmărirea comenzilor, garanție)" NOT marked</t>
   </si>
   <si>
     <t>2)CheckBox "Sunt de acord cu Termeni și condiții și Politica de confidențialitate"</t>
@@ -599,23 +587,6 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>inexistent emailprovider inexistent email domain</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Create new account </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>inexistent emailprovider existent email domain</t>
     </r>
   </si>
@@ -770,15 +741,9 @@
     <t>1)Type"dunca cristina" on *"Parola" and  *"confirmare Parola"</t>
   </si>
   <si>
-    <t>Create new account, password and name have the same content, password is lowercase, name is uppercase</t>
-  </si>
-  <si>
     <t>Reg_#9*</t>
   </si>
   <si>
-    <t>Create new account email length is larger than 1000 letters</t>
-  </si>
-  <si>
     <t>Email: duncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristina@gmail.com</t>
   </si>
   <si>
@@ -786,13 +751,250 @@
   </si>
   <si>
     <t xml:space="preserve">2)Complete other fields with valid data and check mandatory boxex   </t>
+  </si>
+  <si>
+    <t>Reg_#2*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name:"      "                                   
+Other fields valid                </t>
+  </si>
+  <si>
+    <t>1)Type "      " on *Nume si Prenume field</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create new account </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Name Field is whitespace</t>
+    </r>
+  </si>
+  <si>
+    <t>Reg_#2**</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create new account </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Name Field only Symbols</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Name:"")@#$&amp;*"                                   
+Other fields valid                </t>
+  </si>
+  <si>
+    <t>1)Type"")@#$&amp;*" on *Nume si Prenume field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)User should be able to intoruce the symbols </t>
+  </si>
+  <si>
+    <t>Reg_#9**</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create new account </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>email length is larger than 1000 letters</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create new account </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>inexistent email provider inexistent email domain</t>
+    </r>
+  </si>
+  <si>
+    <t>Create new account email name only symbols</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email: "!@#$%^&amp;*(@gmail.com"                               
+Other fields valid     </t>
+  </si>
+  <si>
+    <t>1) Type"!@#$%^&amp;*(@gmail.com" on *"E-mail" field</t>
+  </si>
+  <si>
+    <t>Confirmation "Password:duncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristina"</t>
+  </si>
+  <si>
+    <t>1)Type a word longer than 1000 characters on *Parola and *Confirmare Parola field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password:"duncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristinaduncacristina" </t>
+  </si>
+  <si>
+    <t>Reg_#14**</t>
+  </si>
+  <si>
+    <r>
+      <t>Create new account,</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> password and name have the same content, password is lowercase, name is uppercase</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create new acount, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>password length is larger than 1000 characters</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Create new account</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, mandatory Check box "Sunt de acord ca datele personale colectate în formularul de mai sus să fie folosite pentru crearea unui cont și gestionarea comenzilor (facturare, livrare, urmărirea comenzilor, garanție)"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> NOT marked</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create new account, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">mandatory CheckBox "Sunt de acord cu Termeni și condiții și Politica de confidențialitate" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOT marked</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create new account </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>confirmation password has one different letter from password</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -864,6 +1066,16 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -897,7 +1109,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -1366,11 +1578,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1553,26 +1819,50 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2229,10 +2519,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2B07E3-5E51-4B5D-BCAF-5F148637D0B8}">
-  <dimension ref="A4:I190"/>
+  <dimension ref="A4:I202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2288,7 +2578,7 @@
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="56" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>41</v>
@@ -2314,7 +2604,7 @@
       <c r="B11" s="6"/>
       <c r="C11" s="5"/>
       <c r="D11" s="59" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="58" t="s">
@@ -2416,7 +2706,7 @@
         <v>47</v>
       </c>
       <c r="G16" s="26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H16" s="26" t="s">
         <v>56</v>
@@ -2431,7 +2721,7 @@
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="63" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D17" s="59" t="s">
         <v>59</v>
@@ -2460,7 +2750,7 @@
         <v>60</v>
       </c>
       <c r="G18" s="61" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H18" s="60" t="s">
         <v>56</v>
@@ -2470,45 +2760,43 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="37"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="71"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="92"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="4"/>
       <c r="F19" s="69" t="s">
         <v>45</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="H19" s="70" t="s">
+        <v>106</v>
+      </c>
+      <c r="H19" s="60" t="s">
         <v>56</v>
       </c>
       <c r="I19" s="26" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="64" t="s">
-        <v>62</v>
+    <row r="20" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>150</v>
       </c>
       <c r="B20" s="6"/>
-      <c r="C20" s="72" t="s">
-        <v>143</v>
+      <c r="C20" s="29" t="s">
+        <v>153</v>
       </c>
       <c r="D20" s="59" t="s">
-        <v>89</v>
+        <v>151</v>
       </c>
       <c r="E20" s="65" t="s">
-        <v>64</v>
-      </c>
-      <c r="F20" s="72" t="s">
-        <v>66</v>
-      </c>
-      <c r="G20" s="73" t="s">
-        <v>63</v>
-      </c>
-      <c r="H20" s="70" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="68" t="s">
+        <v>152</v>
+      </c>
+      <c r="G20" s="20"/>
+      <c r="H20" s="60" t="s">
         <v>56</v>
       </c>
       <c r="I20" s="26" t="s">
@@ -2518,16 +2806,16 @@
     <row r="21" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="5"/>
+      <c r="C21" s="29"/>
       <c r="D21" s="7"/>
       <c r="E21" s="6"/>
       <c r="F21" s="68" t="s">
         <v>60</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="H21" s="70" t="s">
+        <v>75</v>
+      </c>
+      <c r="H21" s="60" t="s">
         <v>56</v>
       </c>
       <c r="I21" s="26" t="s">
@@ -2535,16 +2823,16 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="1" t="s">
+      <c r="A22" s="37"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="71"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="69" t="s">
         <v>45</v>
       </c>
       <c r="G22" s="27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H22" s="70" t="s">
         <v>56</v>
@@ -2555,23 +2843,25 @@
     </row>
     <row r="23" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
-        <v>65</v>
+        <v>154</v>
       </c>
       <c r="B23" s="6"/>
-      <c r="C23" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" s="7" t="s">
+      <c r="C23" s="93" t="s">
+        <v>155</v>
+      </c>
+      <c r="D23" s="59" t="s">
+        <v>156</v>
+      </c>
+      <c r="E23" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="F23" s="66" t="s">
-        <v>69</v>
-      </c>
-      <c r="G23" s="20"/>
-      <c r="H23" s="70" t="s">
+      <c r="F23" s="68" t="s">
+        <v>157</v>
+      </c>
+      <c r="G23" s="57" t="s">
+        <v>158</v>
+      </c>
+      <c r="H23" s="60" t="s">
         <v>56</v>
       </c>
       <c r="I23" s="26" t="s">
@@ -2581,23 +2871,23 @@
     <row r="24" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="5"/>
+      <c r="C24" s="93"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="G24" s="61" t="s">
-        <v>72</v>
-      </c>
-      <c r="H24" s="70" t="s">
+      <c r="G24" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="H24" s="60" t="s">
         <v>56</v>
       </c>
       <c r="I24" s="26" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="43"/>
@@ -2607,58 +2897,58 @@
         <v>45</v>
       </c>
       <c r="G25" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="H25" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I25" s="70" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="6" t="s">
-        <v>70</v>
+        <v>106</v>
+      </c>
+      <c r="H25" s="78" t="s">
+        <v>111</v>
+      </c>
+      <c r="I25" s="77" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="64" t="s">
+        <v>62</v>
       </c>
       <c r="B26" s="6"/>
-      <c r="C26" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>58</v>
+      <c r="C26" s="72" t="s">
+        <v>138</v>
+      </c>
+      <c r="D26" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="E26" s="65" t="s">
+        <v>64</v>
       </c>
       <c r="F26" s="72" t="s">
-        <v>75</v>
-      </c>
-      <c r="G26" s="74" t="s">
-        <v>77</v>
+        <v>66</v>
+      </c>
+      <c r="G26" s="91" t="s">
+        <v>63</v>
       </c>
       <c r="H26" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="I26" s="70" t="s">
+      <c r="I26" s="26" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="7"/>
       <c r="E27" s="6"/>
       <c r="F27" s="68" t="s">
         <v>60</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H27" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="I27" s="70" t="s">
+      <c r="I27" s="26" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2668,74 +2958,74 @@
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
-      <c r="F28" s="69" t="s">
+      <c r="F28" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G28" s="27" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H28" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="I28" s="70" t="s">
+      <c r="I28" s="26" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="B29" s="6"/>
-      <c r="C29" s="56" t="s">
-        <v>140</v>
-      </c>
-      <c r="D29" s="75" t="s">
-        <v>88</v>
+      <c r="C29" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F29" s="76" t="s">
-        <v>79</v>
-      </c>
-      <c r="G29" s="27"/>
+      <c r="F29" s="66" t="s">
+        <v>69</v>
+      </c>
+      <c r="G29" s="20"/>
       <c r="H29" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="I29" s="70" t="s">
+      <c r="I29" s="26" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="75"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="G30" s="12" t="s">
-        <v>76</v>
+      <c r="G30" s="61" t="s">
+        <v>71</v>
       </c>
       <c r="H30" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="I30" s="70" t="s">
+      <c r="I30" s="26" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
+      <c r="C31" s="43"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="69" t="s">
         <v>45</v>
       </c>
       <c r="G31" s="27" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="H31" s="70" t="s">
         <v>56</v>
@@ -2746,23 +3036,23 @@
     </row>
     <row r="32" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B32" s="6"/>
-      <c r="C32" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="D32" s="75" t="s">
-        <v>87</v>
+      <c r="C32" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F32" s="76" t="s">
-        <v>90</v>
+      <c r="F32" s="72" t="s">
+        <v>74</v>
       </c>
       <c r="G32" s="74" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H32" s="70" t="s">
         <v>56</v>
@@ -2781,7 +3071,7 @@
         <v>60</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H33" s="70" t="s">
         <v>56</v>
@@ -2800,7 +3090,7 @@
         <v>45</v>
       </c>
       <c r="G34" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H34" s="70" t="s">
         <v>56</v>
@@ -2811,42 +3101,40 @@
     </row>
     <row r="35" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B35" s="6"/>
-      <c r="C35" s="7" t="s">
-        <v>138</v>
+      <c r="C35" s="56" t="s">
+        <v>135</v>
       </c>
       <c r="D35" s="75" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>58</v>
       </c>
       <c r="F35" s="76" t="s">
-        <v>92</v>
-      </c>
-      <c r="G35" s="74" t="s">
-        <v>77</v>
-      </c>
-      <c r="H35" s="77" t="s">
-        <v>93</v>
-      </c>
-      <c r="I35" s="77" t="s">
-        <v>61</v>
+        <v>78</v>
+      </c>
+      <c r="G35" s="27"/>
+      <c r="H35" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I35" s="70" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="75"/>
       <c r="E36" s="6"/>
       <c r="F36" s="68" t="s">
         <v>60</v>
       </c>
       <c r="G36" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H36" s="70" t="s">
         <v>56</v>
@@ -2855,7 +3143,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -2867,38 +3155,38 @@
       <c r="G37" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="H37" s="78" t="s">
-        <v>112</v>
-      </c>
-      <c r="I37" s="77" t="s">
-        <v>61</v>
+      <c r="H37" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I37" s="70" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D38" s="75" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>58</v>
       </c>
       <c r="F38" s="76" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="G38" s="74" t="s">
-        <v>77</v>
-      </c>
-      <c r="H38" s="77" t="s">
-        <v>93</v>
-      </c>
-      <c r="I38" s="77" t="s">
-        <v>61</v>
+        <v>76</v>
+      </c>
+      <c r="H38" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I38" s="70" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -2911,7 +3199,7 @@
         <v>60</v>
       </c>
       <c r="G39" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H39" s="70" t="s">
         <v>56</v>
@@ -2920,7 +3208,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -2930,73 +3218,75 @@
         <v>45</v>
       </c>
       <c r="G40" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="H40" s="78" t="s">
-        <v>94</v>
-      </c>
-      <c r="I40" s="77" t="s">
-        <v>61</v>
+        <v>109</v>
+      </c>
+      <c r="H40" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I40" s="70" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="90" t="s">
-        <v>152</v>
-      </c>
-      <c r="B41" s="91"/>
-      <c r="C41" s="92" t="s">
-        <v>153</v>
-      </c>
-      <c r="D41" s="93" t="s">
-        <v>154</v>
-      </c>
-      <c r="E41" s="92" t="s">
+      <c r="A41" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="6"/>
+      <c r="C41" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D41" s="75" t="s">
+        <v>90</v>
+      </c>
+      <c r="E41" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F41" s="73" t="s">
-        <v>155</v>
+      <c r="F41" s="76" t="s">
+        <v>91</v>
       </c>
       <c r="G41" s="74" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H41" s="77" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I41" s="77" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="64"/>
-      <c r="B42" s="88"/>
-      <c r="C42" s="59"/>
-      <c r="D42" s="89" t="s">
-        <v>122</v>
-      </c>
-      <c r="E42" s="59"/>
-      <c r="F42" s="76" t="s">
-        <v>156</v>
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="68" t="s">
+        <v>60</v>
       </c>
       <c r="G42" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="H42" s="69"/>
-      <c r="I42" s="70"/>
+        <v>75</v>
+      </c>
+      <c r="H42" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I42" s="70" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="43" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="94"/>
-      <c r="B43" s="95"/>
-      <c r="C43" s="96"/>
-      <c r="D43" s="97"/>
-      <c r="E43" s="96"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
       <c r="F43" s="69" t="s">
         <v>45</v>
       </c>
       <c r="G43" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H43" s="78" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I43" s="77" t="s">
         <v>61</v>
@@ -3004,29 +3294,29 @@
     </row>
     <row r="44" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B44" s="6"/>
       <c r="C44" s="7" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="D44" s="75" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>58</v>
       </c>
       <c r="F44" s="76" t="s">
-        <v>98</v>
-      </c>
-      <c r="G44" s="84" t="s">
-        <v>77</v>
-      </c>
-      <c r="H44" s="80" t="s">
-        <v>56</v>
-      </c>
-      <c r="I44" s="70" t="s">
-        <v>28</v>
+        <v>95</v>
+      </c>
+      <c r="G44" s="74" t="s">
+        <v>76</v>
+      </c>
+      <c r="H44" s="77" t="s">
+        <v>92</v>
+      </c>
+      <c r="I44" s="77" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -3039,7 +3329,7 @@
         <v>60</v>
       </c>
       <c r="G45" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H45" s="70" t="s">
         <v>56</v>
@@ -3048,7 +3338,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -3058,51 +3348,55 @@
         <v>45</v>
       </c>
       <c r="G46" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="H46" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I46" s="70" t="s">
-        <v>28</v>
+        <v>109</v>
+      </c>
+      <c r="H46" s="78" t="s">
+        <v>93</v>
+      </c>
+      <c r="I46" s="77" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6" t="s">
+      <c r="A47" s="88" t="s">
+        <v>146</v>
+      </c>
+      <c r="B47" s="60"/>
+      <c r="C47" s="89" t="s">
+        <v>160</v>
+      </c>
+      <c r="D47" s="64" t="s">
         <v>147</v>
       </c>
-      <c r="D47" s="75" t="s">
-        <v>99</v>
-      </c>
-      <c r="E47" s="7" t="s">
+      <c r="E47" s="89" t="s">
         <v>58</v>
       </c>
-      <c r="F47" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="G47" s="22"/>
-      <c r="H47" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I47" s="70" t="s">
-        <v>28</v>
+      <c r="F47" s="73" t="s">
+        <v>148</v>
+      </c>
+      <c r="G47" s="74" t="s">
+        <v>76</v>
+      </c>
+      <c r="H47" s="77" t="s">
+        <v>92</v>
+      </c>
+      <c r="I47" s="77" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="6"/>
+      <c r="A48" s="64"/>
       <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="68" t="s">
-        <v>60</v>
+      <c r="C48" s="59"/>
+      <c r="D48" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E48" s="59"/>
+      <c r="F48" s="76" t="s">
+        <v>149</v>
       </c>
       <c r="G48" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H48" s="70" t="s">
         <v>56</v>
@@ -3111,44 +3405,44 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="4"/>
+    <row r="49" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="90"/>
       <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
+      <c r="C49" s="91"/>
+      <c r="D49" s="83"/>
+      <c r="E49" s="91"/>
       <c r="F49" s="69" t="s">
         <v>45</v>
       </c>
       <c r="G49" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="H49" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I49" s="70" t="s">
-        <v>28</v>
+        <v>109</v>
+      </c>
+      <c r="H49" s="78" t="s">
+        <v>111</v>
+      </c>
+      <c r="I49" s="77" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B50" s="6"/>
-      <c r="C50" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="D50" s="75" t="s">
-        <v>100</v>
-      </c>
-      <c r="E50" s="7" t="s">
+      <c r="A50" s="88" t="s">
+        <v>159</v>
+      </c>
+      <c r="B50" s="60"/>
+      <c r="C50" s="89" t="s">
+        <v>162</v>
+      </c>
+      <c r="D50" s="95" t="s">
+        <v>163</v>
+      </c>
+      <c r="E50" s="89" t="s">
         <v>58</v>
       </c>
-      <c r="F50" s="7" t="s">
-        <v>102</v>
+      <c r="F50" s="94" t="s">
+        <v>164</v>
       </c>
       <c r="G50" s="74" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
       <c r="H50" s="70" t="s">
         <v>56</v>
@@ -3158,16 +3452,16 @@
       </c>
     </row>
     <row r="51" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="6"/>
+      <c r="A51" s="64"/>
       <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="68" t="s">
-        <v>60</v>
+      <c r="C51" s="59"/>
+      <c r="D51" s="81"/>
+      <c r="E51" s="59"/>
+      <c r="F51" s="76" t="s">
+        <v>149</v>
       </c>
       <c r="G51" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H51" s="70" t="s">
         <v>56</v>
@@ -3177,16 +3471,16 @@
       </c>
     </row>
     <row r="52" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="4"/>
+      <c r="A52" s="90"/>
       <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
+      <c r="C52" s="91"/>
+      <c r="D52" s="83"/>
+      <c r="E52" s="91"/>
       <c r="F52" s="69" t="s">
         <v>45</v>
       </c>
       <c r="G52" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H52" s="70" t="s">
         <v>56</v>
@@ -3197,25 +3491,25 @@
     </row>
     <row r="53" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B53" s="6"/>
-      <c r="C53" s="6" t="s">
-        <v>134</v>
+      <c r="C53" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="D53" s="75" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="E53" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F53" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="G53" s="74" t="s">
-        <v>103</v>
-      </c>
-      <c r="H53" s="70" t="s">
+      <c r="F53" s="76" t="s">
+        <v>97</v>
+      </c>
+      <c r="G53" s="84" t="s">
+        <v>76</v>
+      </c>
+      <c r="H53" s="80" t="s">
         <v>56</v>
       </c>
       <c r="I53" s="70" t="s">
@@ -3232,7 +3526,7 @@
         <v>60</v>
       </c>
       <c r="G54" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H54" s="70" t="s">
         <v>56</v>
@@ -3251,7 +3545,7 @@
         <v>45</v>
       </c>
       <c r="G55" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H55" s="70" t="s">
         <v>56</v>
@@ -3260,26 +3554,24 @@
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="6" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="B56" s="6"/>
-      <c r="C56" s="7" t="s">
-        <v>133</v>
+      <c r="C56" s="6" t="s">
+        <v>142</v>
       </c>
       <c r="D56" s="75" t="s">
-        <v>127</v>
+        <v>98</v>
       </c>
       <c r="E56" s="7" t="s">
         <v>58</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G56" s="74" t="s">
-        <v>103</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="G56" s="22"/>
       <c r="H56" s="70" t="s">
         <v>56</v>
       </c>
@@ -3297,7 +3589,7 @@
         <v>60</v>
       </c>
       <c r="G57" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H57" s="70" t="s">
         <v>56</v>
@@ -3316,7 +3608,7 @@
         <v>45</v>
       </c>
       <c r="G58" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H58" s="70" t="s">
         <v>56</v>
@@ -3325,44 +3617,44 @@
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="87" t="s">
-        <v>148</v>
-      </c>
-      <c r="B59" s="60"/>
-      <c r="C59" s="61" t="s">
-        <v>151</v>
+    <row r="59" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B59" s="6"/>
+      <c r="C59" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="D59" s="75" t="s">
-        <v>149</v>
+        <v>99</v>
       </c>
       <c r="E59" s="7" t="s">
         <v>58</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>150</v>
+        <v>101</v>
       </c>
       <c r="G59" s="74" t="s">
-        <v>103</v>
-      </c>
-      <c r="H59" s="85" t="s">
-        <v>93</v>
-      </c>
-      <c r="I59" s="85" t="s">
-        <v>61</v>
+        <v>102</v>
+      </c>
+      <c r="H59" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I59" s="70" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
-      <c r="C60" s="7"/>
-      <c r="D60" s="75"/>
-      <c r="E60" s="7"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
       <c r="F60" s="68" t="s">
         <v>60</v>
       </c>
       <c r="G60" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H60" s="70" t="s">
         <v>56</v>
@@ -3371,7 +3663,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="1:9" s="86" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -3381,40 +3673,40 @@
         <v>45</v>
       </c>
       <c r="G61" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="H61" s="78" t="s">
-        <v>94</v>
-      </c>
-      <c r="I61" s="77" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+      <c r="H61" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I61" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="6" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="B62" s="6"/>
-      <c r="C62" s="7" t="s">
-        <v>132</v>
+      <c r="C62" s="6" t="s">
+        <v>130</v>
       </c>
       <c r="D62" s="75" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="E62" s="7" t="s">
         <v>58</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="G62" s="84" t="s">
-        <v>103</v>
-      </c>
-      <c r="H62" s="85" t="s">
-        <v>93</v>
-      </c>
-      <c r="I62" s="85" t="s">
-        <v>61</v>
+        <v>104</v>
+      </c>
+      <c r="G62" s="74" t="s">
+        <v>102</v>
+      </c>
+      <c r="H62" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I62" s="70" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -3427,7 +3719,7 @@
         <v>60</v>
       </c>
       <c r="G63" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H63" s="70" t="s">
         <v>56</v>
@@ -3436,7 +3728,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -3446,34 +3738,34 @@
         <v>45</v>
       </c>
       <c r="G64" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="H64" s="78" t="s">
-        <v>94</v>
-      </c>
-      <c r="I64" s="77" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+      <c r="H64" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I64" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="6" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B65" s="6"/>
       <c r="C65" s="7" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="D65" s="75" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="E65" s="7" t="s">
         <v>58</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G65" s="74" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H65" s="70" t="s">
         <v>56</v>
@@ -3492,7 +3784,7 @@
         <v>60</v>
       </c>
       <c r="G66" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H66" s="70" t="s">
         <v>56</v>
@@ -3511,7 +3803,7 @@
         <v>45</v>
       </c>
       <c r="G67" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H67" s="70" t="s">
         <v>56</v>
@@ -3520,44 +3812,44 @@
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B68" s="6"/>
-      <c r="C68" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>122</v>
+    <row r="68" spans="1:9" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="87" t="s">
+        <v>143</v>
+      </c>
+      <c r="B68" s="60"/>
+      <c r="C68" s="61" t="s">
+        <v>170</v>
+      </c>
+      <c r="D68" s="75" t="s">
+        <v>144</v>
       </c>
       <c r="E68" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F68" s="79" t="s">
-        <v>123</v>
-      </c>
-      <c r="G68" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="H68" s="80" t="s">
-        <v>56</v>
-      </c>
-      <c r="I68" s="80" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F68" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G68" s="74" t="s">
+        <v>102</v>
+      </c>
+      <c r="H68" s="85" t="s">
+        <v>92</v>
+      </c>
+      <c r="I68" s="85" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="6"/>
       <c r="B69" s="6"/>
-      <c r="C69" s="6"/>
-      <c r="D69" s="6"/>
-      <c r="E69" s="6"/>
-      <c r="F69" s="61" t="s">
-        <v>131</v>
-      </c>
-      <c r="G69" s="4" t="s">
-        <v>125</v>
+      <c r="C69" s="7"/>
+      <c r="D69" s="75"/>
+      <c r="E69" s="7"/>
+      <c r="F69" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="G69" s="12" t="s">
+        <v>75</v>
       </c>
       <c r="H69" s="70" t="s">
         <v>56</v>
@@ -3566,221 +3858,355 @@
         <v>28</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="4"/>
-      <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
-      <c r="D70" s="4"/>
-      <c r="E70" s="4"/>
-      <c r="F70" s="69" t="s">
+    <row r="70" spans="1:9" s="86" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="6"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="G70" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="H70" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I70" s="70" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" ht="87" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="81" t="s">
-        <v>128</v>
-      </c>
-      <c r="B71" s="81"/>
-      <c r="C71" s="82" t="s">
-        <v>129</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="E71" s="82" t="s">
+      <c r="G70" s="61" t="s">
+        <v>109</v>
+      </c>
+      <c r="H70" s="105" t="s">
+        <v>93</v>
+      </c>
+      <c r="I70" s="98" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" s="96" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="99" t="s">
+        <v>169</v>
+      </c>
+      <c r="B71" s="18"/>
+      <c r="C71" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="D71" s="106" t="s">
+        <v>168</v>
+      </c>
+      <c r="E71" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="F71" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="G71" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="H71" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I71" s="70" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="81"/>
-      <c r="B72" s="81"/>
-      <c r="C72" s="81"/>
-      <c r="D72" s="81"/>
-      <c r="E72" s="81"/>
-      <c r="F72" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="G72" s="4" t="s">
-        <v>125</v>
+      <c r="F71" s="107" t="s">
+        <v>166</v>
+      </c>
+      <c r="G71" s="101" t="s">
+        <v>102</v>
+      </c>
+      <c r="H71" s="102" t="s">
+        <v>92</v>
+      </c>
+      <c r="I71" s="103" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" s="96" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="24"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="64" t="s">
+        <v>165</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="F72" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="G72" s="12" t="s">
+        <v>75</v>
       </c>
       <c r="H72" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="I72" s="70" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="83"/>
-      <c r="B73" s="83"/>
-      <c r="C73" s="83"/>
-      <c r="D73" s="83"/>
-      <c r="E73" s="83"/>
+      <c r="I72" s="28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" s="96" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="36"/>
+      <c r="B73" s="37"/>
+      <c r="C73" s="37"/>
+      <c r="D73" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="E73" s="37"/>
       <c r="F73" s="69" t="s">
         <v>45</v>
       </c>
       <c r="G73" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="H73" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I73" s="70" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74" s="6"/>
-      <c r="B74" s="6"/>
-      <c r="C74" s="6"/>
-      <c r="D74" s="6"/>
-      <c r="E74" s="6"/>
-      <c r="F74" s="6"/>
-      <c r="G74" s="6"/>
-      <c r="H74" s="6"/>
-      <c r="I74" s="6"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A75" s="6"/>
+        <v>109</v>
+      </c>
+      <c r="H73" s="85" t="s">
+        <v>92</v>
+      </c>
+      <c r="I73" s="104" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="99" t="s">
+        <v>113</v>
+      </c>
+      <c r="B74" s="18"/>
+      <c r="C74" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="D74" s="100" t="s">
+        <v>123</v>
+      </c>
+      <c r="E74" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="F74" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="G74" s="101" t="s">
+        <v>102</v>
+      </c>
+      <c r="H74" s="102" t="s">
+        <v>92</v>
+      </c>
+      <c r="I74" s="103" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="24"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
       <c r="D75" s="6"/>
       <c r="E75" s="6"/>
-      <c r="F75" s="6"/>
-      <c r="G75" s="6"/>
-      <c r="H75" s="6"/>
-      <c r="I75" s="6"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A76" s="6"/>
-      <c r="B76" s="6"/>
-      <c r="C76" s="6"/>
-      <c r="D76" s="6"/>
-      <c r="E76" s="6"/>
-      <c r="F76" s="6"/>
-      <c r="G76" s="6"/>
-      <c r="H76" s="6"/>
-      <c r="I76" s="6"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A77" s="6"/>
+      <c r="F75" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="G75" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="H75" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I75" s="28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="36"/>
+      <c r="B76" s="37"/>
+      <c r="C76" s="37"/>
+      <c r="D76" s="37"/>
+      <c r="E76" s="37"/>
+      <c r="F76" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="G76" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="H76" s="78" t="s">
+        <v>93</v>
+      </c>
+      <c r="I76" s="104" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="6" t="s">
+        <v>115</v>
+      </c>
       <c r="B77" s="6"/>
-      <c r="C77" s="6"/>
-      <c r="D77" s="6"/>
-      <c r="E77" s="6"/>
-      <c r="F77" s="6"/>
-      <c r="G77" s="6"/>
-      <c r="H77" s="6"/>
-      <c r="I77" s="6"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C77" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="D77" s="75" t="s">
+        <v>116</v>
+      </c>
+      <c r="E77" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="G77" s="84" t="s">
+        <v>102</v>
+      </c>
+      <c r="H77" s="80" t="s">
+        <v>56</v>
+      </c>
+      <c r="I77" s="80" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="6"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
       <c r="E78" s="6"/>
-      <c r="F78" s="6"/>
-      <c r="G78" s="6"/>
-      <c r="H78" s="6"/>
-      <c r="I78" s="6"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" s="6"/>
-      <c r="B79" s="6"/>
-      <c r="C79" s="6"/>
-      <c r="D79" s="6"/>
-      <c r="E79" s="6"/>
-      <c r="F79" s="6"/>
-      <c r="G79" s="6"/>
-      <c r="H79" s="6"/>
-      <c r="I79" s="6"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A80" s="6"/>
+      <c r="F78" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="G78" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="H78" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I78" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="G79" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="H79" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I79" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="6" t="s">
+        <v>118</v>
+      </c>
       <c r="B80" s="6"/>
-      <c r="C80" s="6"/>
-      <c r="D80" s="6"/>
-      <c r="E80" s="6"/>
-      <c r="F80" s="6"/>
-      <c r="G80" s="6"/>
-      <c r="H80" s="6"/>
-      <c r="I80" s="6"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C80" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E80" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F80" s="79" t="s">
+        <v>120</v>
+      </c>
+      <c r="G80" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="H80" s="80" t="s">
+        <v>56</v>
+      </c>
+      <c r="I80" s="80" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="6"/>
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
       <c r="D81" s="6"/>
       <c r="E81" s="6"/>
-      <c r="F81" s="6"/>
-      <c r="G81" s="6"/>
-      <c r="H81" s="6"/>
-      <c r="I81" s="6"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A82" s="6"/>
-      <c r="B82" s="6"/>
-      <c r="C82" s="6"/>
-      <c r="D82" s="6"/>
-      <c r="E82" s="6"/>
-      <c r="F82" s="6"/>
-      <c r="G82" s="6"/>
-      <c r="H82" s="6"/>
-      <c r="I82" s="6"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A83" s="6"/>
-      <c r="B83" s="6"/>
-      <c r="C83" s="6"/>
-      <c r="D83" s="6"/>
-      <c r="E83" s="6"/>
-      <c r="F83" s="6"/>
-      <c r="G83" s="6"/>
-      <c r="H83" s="6"/>
-      <c r="I83" s="6"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" s="6"/>
-      <c r="B84" s="6"/>
-      <c r="C84" s="6"/>
-      <c r="D84" s="6"/>
-      <c r="E84" s="6"/>
-      <c r="F84" s="6"/>
-      <c r="G84" s="6"/>
-      <c r="H84" s="6"/>
-      <c r="I84" s="6"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" s="6"/>
-      <c r="B85" s="6"/>
-      <c r="C85" s="6"/>
-      <c r="D85" s="6"/>
-      <c r="E85" s="6"/>
-      <c r="F85" s="6"/>
-      <c r="G85" s="6"/>
-      <c r="H85" s="6"/>
-      <c r="I85" s="6"/>
+      <c r="F81" s="61" t="s">
+        <v>127</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="H81" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I81" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="4"/>
+      <c r="B82" s="4"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="G82" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="H82" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I82" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="81" t="s">
+        <v>125</v>
+      </c>
+      <c r="B83" s="81"/>
+      <c r="C83" s="97" t="s">
+        <v>172</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E83" s="82" t="s">
+        <v>58</v>
+      </c>
+      <c r="F83" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="G83" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="H83" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I83" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="81"/>
+      <c r="B84" s="81"/>
+      <c r="C84" s="81"/>
+      <c r="D84" s="81"/>
+      <c r="E84" s="81"/>
+      <c r="F84" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="G84" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="H84" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I84" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="83"/>
+      <c r="B85" s="83"/>
+      <c r="C85" s="83"/>
+      <c r="D85" s="83"/>
+      <c r="E85" s="83"/>
+      <c r="F85" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="G85" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="H85" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I85" s="70" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="6"/>
@@ -4937,6 +5363,138 @@
       <c r="H190" s="6"/>
       <c r="I190" s="6"/>
     </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A191" s="6"/>
+      <c r="B191" s="6"/>
+      <c r="C191" s="6"/>
+      <c r="D191" s="6"/>
+      <c r="E191" s="6"/>
+      <c r="F191" s="6"/>
+      <c r="G191" s="6"/>
+      <c r="H191" s="6"/>
+      <c r="I191" s="6"/>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A192" s="6"/>
+      <c r="B192" s="6"/>
+      <c r="C192" s="6"/>
+      <c r="D192" s="6"/>
+      <c r="E192" s="6"/>
+      <c r="F192" s="6"/>
+      <c r="G192" s="6"/>
+      <c r="H192" s="6"/>
+      <c r="I192" s="6"/>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A193" s="6"/>
+      <c r="B193" s="6"/>
+      <c r="C193" s="6"/>
+      <c r="D193" s="6"/>
+      <c r="E193" s="6"/>
+      <c r="F193" s="6"/>
+      <c r="G193" s="6"/>
+      <c r="H193" s="6"/>
+      <c r="I193" s="6"/>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A194" s="6"/>
+      <c r="B194" s="6"/>
+      <c r="C194" s="6"/>
+      <c r="D194" s="6"/>
+      <c r="E194" s="6"/>
+      <c r="F194" s="6"/>
+      <c r="G194" s="6"/>
+      <c r="H194" s="6"/>
+      <c r="I194" s="6"/>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A195" s="6"/>
+      <c r="B195" s="6"/>
+      <c r="C195" s="6"/>
+      <c r="D195" s="6"/>
+      <c r="E195" s="6"/>
+      <c r="F195" s="6"/>
+      <c r="G195" s="6"/>
+      <c r="H195" s="6"/>
+      <c r="I195" s="6"/>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A196" s="6"/>
+      <c r="B196" s="6"/>
+      <c r="C196" s="6"/>
+      <c r="D196" s="6"/>
+      <c r="E196" s="6"/>
+      <c r="F196" s="6"/>
+      <c r="G196" s="6"/>
+      <c r="H196" s="6"/>
+      <c r="I196" s="6"/>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A197" s="6"/>
+      <c r="B197" s="6"/>
+      <c r="C197" s="6"/>
+      <c r="D197" s="6"/>
+      <c r="E197" s="6"/>
+      <c r="F197" s="6"/>
+      <c r="G197" s="6"/>
+      <c r="H197" s="6"/>
+      <c r="I197" s="6"/>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A198" s="6"/>
+      <c r="B198" s="6"/>
+      <c r="C198" s="6"/>
+      <c r="D198" s="6"/>
+      <c r="E198" s="6"/>
+      <c r="F198" s="6"/>
+      <c r="G198" s="6"/>
+      <c r="H198" s="6"/>
+      <c r="I198" s="6"/>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A199" s="6"/>
+      <c r="B199" s="6"/>
+      <c r="C199" s="6"/>
+      <c r="D199" s="6"/>
+      <c r="E199" s="6"/>
+      <c r="F199" s="6"/>
+      <c r="G199" s="6"/>
+      <c r="H199" s="6"/>
+      <c r="I199" s="6"/>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A200" s="6"/>
+      <c r="B200" s="6"/>
+      <c r="C200" s="6"/>
+      <c r="D200" s="6"/>
+      <c r="E200" s="6"/>
+      <c r="F200" s="6"/>
+      <c r="G200" s="6"/>
+      <c r="H200" s="6"/>
+      <c r="I200" s="6"/>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A201" s="6"/>
+      <c r="B201" s="6"/>
+      <c r="C201" s="6"/>
+      <c r="D201" s="6"/>
+      <c r="E201" s="6"/>
+      <c r="F201" s="6"/>
+      <c r="G201" s="6"/>
+      <c r="H201" s="6"/>
+      <c r="I201" s="6"/>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A202" s="6"/>
+      <c r="B202" s="6"/>
+      <c r="C202" s="6"/>
+      <c r="D202" s="6"/>
+      <c r="E202" s="6"/>
+      <c r="F202" s="6"/>
+      <c r="G202" s="6"/>
+      <c r="H202" s="6"/>
+      <c r="I202" s="6"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added tests for login page
</commit_message>
<xml_diff>
--- a/QA/Selenium/Test Cases.xlsx
+++ b/QA/Selenium/Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sorin\Desktop\Junior\Modul2\Json.Start\QA\Selenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384F2229-D975-45A7-BC31-70FCFA4A5D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA952BAF-7097-43A9-82F9-B37ACD764621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1077,7 +1077,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1105,6 +1105,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1636,7 +1654,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1762,9 +1780,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1832,14 +1847,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1861,6 +1874,37 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2521,8 +2565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2B07E3-5E51-4B5D-BCAF-5F148637D0B8}">
   <dimension ref="A4:I202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2539,7 +2583,7 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="66" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2577,7 +2621,7 @@
         <v>40</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="56" t="s">
+      <c r="C10" s="106" t="s">
         <v>140</v>
       </c>
       <c r="D10" s="7" t="s">
@@ -2716,20 +2760,20 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="64" t="s">
+      <c r="A17" s="63" t="s">
         <v>57</v>
       </c>
       <c r="B17" s="6"/>
-      <c r="C17" s="63" t="s">
+      <c r="C17" s="107" t="s">
         <v>139</v>
       </c>
       <c r="D17" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="65" t="s">
+      <c r="E17" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="F17" s="66" t="s">
+      <c r="F17" s="65" t="s">
         <v>68</v>
       </c>
       <c r="G17" s="20"/>
@@ -2746,7 +2790,7 @@
       <c r="C18" s="6"/>
       <c r="D18" s="7"/>
       <c r="E18" s="6"/>
-      <c r="F18" s="68" t="s">
+      <c r="F18" s="67" t="s">
         <v>60</v>
       </c>
       <c r="G18" s="61" t="s">
@@ -2762,10 +2806,10 @@
     <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="92"/>
+      <c r="C19" s="91"/>
       <c r="D19" s="12"/>
       <c r="E19" s="4"/>
-      <c r="F19" s="69" t="s">
+      <c r="F19" s="68" t="s">
         <v>45</v>
       </c>
       <c r="G19" s="27" t="s">
@@ -2783,16 +2827,16 @@
         <v>150</v>
       </c>
       <c r="B20" s="6"/>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="108" t="s">
         <v>153</v>
       </c>
       <c r="D20" s="59" t="s">
         <v>151</v>
       </c>
-      <c r="E20" s="65" t="s">
+      <c r="E20" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="F20" s="68" t="s">
+      <c r="F20" s="67" t="s">
         <v>152</v>
       </c>
       <c r="G20" s="20"/>
@@ -2809,7 +2853,7 @@
       <c r="C21" s="29"/>
       <c r="D21" s="7"/>
       <c r="E21" s="6"/>
-      <c r="F21" s="68" t="s">
+      <c r="F21" s="67" t="s">
         <v>60</v>
       </c>
       <c r="G21" s="12" t="s">
@@ -2825,16 +2869,16 @@
     <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="37"/>
       <c r="B22" s="37"/>
-      <c r="C22" s="71"/>
+      <c r="C22" s="70"/>
       <c r="D22" s="37"/>
       <c r="E22" s="37"/>
-      <c r="F22" s="69" t="s">
+      <c r="F22" s="68" t="s">
         <v>45</v>
       </c>
       <c r="G22" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="H22" s="70" t="s">
+      <c r="H22" s="69" t="s">
         <v>56</v>
       </c>
       <c r="I22" s="26" t="s">
@@ -2846,16 +2890,16 @@
         <v>154</v>
       </c>
       <c r="B23" s="6"/>
-      <c r="C23" s="93" t="s">
+      <c r="C23" s="105" t="s">
         <v>155</v>
       </c>
       <c r="D23" s="59" t="s">
         <v>156</v>
       </c>
-      <c r="E23" s="65" t="s">
+      <c r="E23" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="F23" s="68" t="s">
+      <c r="F23" s="67" t="s">
         <v>157</v>
       </c>
       <c r="G23" s="57" t="s">
@@ -2871,10 +2915,10 @@
     <row r="24" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="93"/>
+      <c r="C24" s="5"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
-      <c r="F24" s="68" t="s">
+      <c r="F24" s="67" t="s">
         <v>60</v>
       </c>
       <c r="G24" s="12" t="s">
@@ -2893,40 +2937,40 @@
       <c r="C25" s="43"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
-      <c r="F25" s="69" t="s">
+      <c r="F25" s="68" t="s">
         <v>45</v>
       </c>
       <c r="G25" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="H25" s="78" t="s">
+      <c r="H25" s="77" t="s">
         <v>111</v>
       </c>
-      <c r="I25" s="77" t="s">
+      <c r="I25" s="76" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="64" t="s">
+      <c r="A26" s="63" t="s">
         <v>62</v>
       </c>
       <c r="B26" s="6"/>
-      <c r="C26" s="72" t="s">
+      <c r="C26" s="109" t="s">
         <v>138</v>
       </c>
       <c r="D26" s="59" t="s">
         <v>88</v>
       </c>
-      <c r="E26" s="65" t="s">
+      <c r="E26" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="F26" s="72" t="s">
+      <c r="F26" s="71" t="s">
         <v>66</v>
       </c>
-      <c r="G26" s="91" t="s">
+      <c r="G26" s="90" t="s">
         <v>63</v>
       </c>
-      <c r="H26" s="70" t="s">
+      <c r="H26" s="69" t="s">
         <v>56</v>
       </c>
       <c r="I26" s="26" t="s">
@@ -2939,13 +2983,13 @@
       <c r="C27" s="5"/>
       <c r="D27" s="7"/>
       <c r="E27" s="6"/>
-      <c r="F27" s="68" t="s">
+      <c r="F27" s="67" t="s">
         <v>60</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="H27" s="70" t="s">
+      <c r="H27" s="69" t="s">
         <v>56</v>
       </c>
       <c r="I27" s="26" t="s">
@@ -2964,7 +3008,7 @@
       <c r="G28" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="H28" s="70" t="s">
+      <c r="H28" s="69" t="s">
         <v>56</v>
       </c>
       <c r="I28" s="26" t="s">
@@ -2976,7 +3020,7 @@
         <v>65</v>
       </c>
       <c r="B29" s="6"/>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="110" t="s">
         <v>137</v>
       </c>
       <c r="D29" s="7" t="s">
@@ -2985,11 +3029,11 @@
       <c r="E29" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F29" s="66" t="s">
+      <c r="F29" s="65" t="s">
         <v>69</v>
       </c>
       <c r="G29" s="20"/>
-      <c r="H29" s="70" t="s">
+      <c r="H29" s="69" t="s">
         <v>56</v>
       </c>
       <c r="I29" s="26" t="s">
@@ -3002,13 +3046,13 @@
       <c r="C30" s="5"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
-      <c r="F30" s="68" t="s">
+      <c r="F30" s="67" t="s">
         <v>60</v>
       </c>
       <c r="G30" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="H30" s="70" t="s">
+      <c r="H30" s="69" t="s">
         <v>56</v>
       </c>
       <c r="I30" s="26" t="s">
@@ -3021,16 +3065,16 @@
       <c r="C31" s="43"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
-      <c r="F31" s="69" t="s">
+      <c r="F31" s="68" t="s">
         <v>45</v>
       </c>
       <c r="G31" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="H31" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I31" s="70" t="s">
+      <c r="H31" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I31" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3039,7 +3083,7 @@
         <v>70</v>
       </c>
       <c r="B32" s="6"/>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="110" t="s">
         <v>136</v>
       </c>
       <c r="D32" s="7" t="s">
@@ -3048,16 +3092,16 @@
       <c r="E32" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F32" s="72" t="s">
+      <c r="F32" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="G32" s="74" t="s">
+      <c r="G32" s="73" t="s">
         <v>76</v>
       </c>
-      <c r="H32" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I32" s="70" t="s">
+      <c r="H32" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I32" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3067,16 +3111,16 @@
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
-      <c r="F33" s="68" t="s">
+      <c r="F33" s="67" t="s">
         <v>60</v>
       </c>
       <c r="G33" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="H33" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I33" s="70" t="s">
+      <c r="H33" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I33" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3086,16 +3130,16 @@
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
-      <c r="F34" s="69" t="s">
+      <c r="F34" s="68" t="s">
         <v>45</v>
       </c>
       <c r="G34" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="H34" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I34" s="70" t="s">
+      <c r="H34" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I34" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3104,23 +3148,23 @@
         <v>77</v>
       </c>
       <c r="B35" s="6"/>
-      <c r="C35" s="56" t="s">
+      <c r="C35" s="111" t="s">
         <v>135</v>
       </c>
-      <c r="D35" s="75" t="s">
+      <c r="D35" s="74" t="s">
         <v>87</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F35" s="76" t="s">
+      <c r="F35" s="75" t="s">
         <v>78</v>
       </c>
       <c r="G35" s="27"/>
-      <c r="H35" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I35" s="70" t="s">
+      <c r="H35" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I35" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3128,18 +3172,18 @@
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="56"/>
-      <c r="D36" s="75"/>
+      <c r="D36" s="74"/>
       <c r="E36" s="6"/>
-      <c r="F36" s="68" t="s">
+      <c r="F36" s="67" t="s">
         <v>60</v>
       </c>
       <c r="G36" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="H36" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I36" s="70" t="s">
+      <c r="H36" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I36" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3149,16 +3193,16 @@
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
-      <c r="F37" s="69" t="s">
+      <c r="F37" s="68" t="s">
         <v>45</v>
       </c>
       <c r="G37" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="H37" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I37" s="70" t="s">
+      <c r="H37" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I37" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3167,25 +3211,25 @@
         <v>79</v>
       </c>
       <c r="B38" s="6"/>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="112" t="s">
         <v>134</v>
       </c>
-      <c r="D38" s="75" t="s">
+      <c r="D38" s="74" t="s">
         <v>86</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F38" s="76" t="s">
+      <c r="F38" s="75" t="s">
         <v>89</v>
       </c>
-      <c r="G38" s="74" t="s">
+      <c r="G38" s="73" t="s">
         <v>76</v>
       </c>
-      <c r="H38" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I38" s="70" t="s">
+      <c r="H38" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I38" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3195,16 +3239,16 @@
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
-      <c r="F39" s="68" t="s">
+      <c r="F39" s="67" t="s">
         <v>60</v>
       </c>
       <c r="G39" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="H39" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I39" s="70" t="s">
+      <c r="H39" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I39" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3214,16 +3258,16 @@
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
-      <c r="F40" s="69" t="s">
+      <c r="F40" s="68" t="s">
         <v>45</v>
       </c>
       <c r="G40" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="H40" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I40" s="70" t="s">
+      <c r="H40" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I40" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3232,25 +3276,25 @@
         <v>80</v>
       </c>
       <c r="B41" s="6"/>
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="112" t="s">
         <v>133</v>
       </c>
-      <c r="D41" s="75" t="s">
+      <c r="D41" s="74" t="s">
         <v>90</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F41" s="76" t="s">
+      <c r="F41" s="75" t="s">
         <v>91</v>
       </c>
-      <c r="G41" s="74" t="s">
+      <c r="G41" s="73" t="s">
         <v>76</v>
       </c>
-      <c r="H41" s="77" t="s">
+      <c r="H41" s="76" t="s">
         <v>92</v>
       </c>
-      <c r="I41" s="77" t="s">
+      <c r="I41" s="76" t="s">
         <v>61</v>
       </c>
     </row>
@@ -3260,16 +3304,16 @@
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
-      <c r="F42" s="68" t="s">
+      <c r="F42" s="67" t="s">
         <v>60</v>
       </c>
       <c r="G42" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="H42" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I42" s="70" t="s">
+      <c r="H42" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I42" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3279,16 +3323,16 @@
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
-      <c r="F43" s="69" t="s">
+      <c r="F43" s="68" t="s">
         <v>45</v>
       </c>
       <c r="G43" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="H43" s="78" t="s">
+      <c r="H43" s="77" t="s">
         <v>111</v>
       </c>
-      <c r="I43" s="77" t="s">
+      <c r="I43" s="76" t="s">
         <v>61</v>
       </c>
     </row>
@@ -3297,25 +3341,25 @@
         <v>81</v>
       </c>
       <c r="B44" s="6"/>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="112" t="s">
         <v>161</v>
       </c>
-      <c r="D44" s="75" t="s">
+      <c r="D44" s="74" t="s">
         <v>94</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F44" s="76" t="s">
+      <c r="F44" s="75" t="s">
         <v>95</v>
       </c>
-      <c r="G44" s="74" t="s">
+      <c r="G44" s="73" t="s">
         <v>76</v>
       </c>
-      <c r="H44" s="77" t="s">
+      <c r="H44" s="76" t="s">
         <v>92</v>
       </c>
-      <c r="I44" s="77" t="s">
+      <c r="I44" s="76" t="s">
         <v>61</v>
       </c>
     </row>
@@ -3325,16 +3369,16 @@
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
-      <c r="F45" s="68" t="s">
+      <c r="F45" s="67" t="s">
         <v>60</v>
       </c>
       <c r="G45" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="H45" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I45" s="70" t="s">
+      <c r="H45" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I45" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3344,148 +3388,148 @@
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
-      <c r="F46" s="69" t="s">
+      <c r="F46" s="68" t="s">
         <v>45</v>
       </c>
       <c r="G46" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="H46" s="78" t="s">
+      <c r="H46" s="77" t="s">
         <v>93</v>
       </c>
-      <c r="I46" s="77" t="s">
+      <c r="I46" s="76" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="88" t="s">
+      <c r="A47" s="87" t="s">
         <v>146</v>
       </c>
       <c r="B47" s="60"/>
-      <c r="C47" s="89" t="s">
+      <c r="C47" s="113" t="s">
         <v>160</v>
       </c>
-      <c r="D47" s="64" t="s">
+      <c r="D47" s="63" t="s">
         <v>147</v>
       </c>
-      <c r="E47" s="89" t="s">
+      <c r="E47" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="F47" s="73" t="s">
+      <c r="F47" s="72" t="s">
         <v>148</v>
       </c>
-      <c r="G47" s="74" t="s">
+      <c r="G47" s="73" t="s">
         <v>76</v>
       </c>
-      <c r="H47" s="77" t="s">
+      <c r="H47" s="76" t="s">
         <v>92</v>
       </c>
-      <c r="I47" s="77" t="s">
+      <c r="I47" s="76" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="64"/>
+      <c r="A48" s="63"/>
       <c r="B48" s="6"/>
       <c r="C48" s="59"/>
       <c r="D48" s="6" t="s">
         <v>119</v>
       </c>
       <c r="E48" s="59"/>
-      <c r="F48" s="76" t="s">
+      <c r="F48" s="75" t="s">
         <v>149</v>
       </c>
       <c r="G48" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="H48" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I48" s="70" t="s">
+      <c r="H48" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I48" s="69" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="90"/>
+      <c r="A49" s="89"/>
       <c r="B49" s="4"/>
-      <c r="C49" s="91"/>
-      <c r="D49" s="83"/>
-      <c r="E49" s="91"/>
-      <c r="F49" s="69" t="s">
+      <c r="C49" s="90"/>
+      <c r="D49" s="82"/>
+      <c r="E49" s="90"/>
+      <c r="F49" s="68" t="s">
         <v>45</v>
       </c>
       <c r="G49" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="H49" s="78" t="s">
+      <c r="H49" s="77" t="s">
         <v>111</v>
       </c>
-      <c r="I49" s="77" t="s">
+      <c r="I49" s="76" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="88" t="s">
+      <c r="A50" s="87" t="s">
         <v>159</v>
       </c>
       <c r="B50" s="60"/>
-      <c r="C50" s="89" t="s">
+      <c r="C50" s="113" t="s">
         <v>162</v>
       </c>
-      <c r="D50" s="95" t="s">
+      <c r="D50" s="93" t="s">
         <v>163</v>
       </c>
-      <c r="E50" s="89" t="s">
+      <c r="E50" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="F50" s="94" t="s">
+      <c r="F50" s="92" t="s">
         <v>164</v>
       </c>
-      <c r="G50" s="74" t="s">
+      <c r="G50" s="73" t="s">
         <v>76</v>
       </c>
-      <c r="H50" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I50" s="70" t="s">
+      <c r="H50" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I50" s="69" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="64"/>
+      <c r="A51" s="63"/>
       <c r="B51" s="6"/>
       <c r="C51" s="59"/>
-      <c r="D51" s="81"/>
+      <c r="D51" s="80"/>
       <c r="E51" s="59"/>
-      <c r="F51" s="76" t="s">
+      <c r="F51" s="75" t="s">
         <v>149</v>
       </c>
       <c r="G51" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="H51" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I51" s="70" t="s">
+      <c r="H51" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I51" s="69" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="90"/>
+      <c r="A52" s="89"/>
       <c r="B52" s="4"/>
-      <c r="C52" s="91"/>
-      <c r="D52" s="83"/>
-      <c r="E52" s="91"/>
-      <c r="F52" s="69" t="s">
+      <c r="C52" s="90"/>
+      <c r="D52" s="82"/>
+      <c r="E52" s="90"/>
+      <c r="F52" s="68" t="s">
         <v>45</v>
       </c>
       <c r="G52" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="H52" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I52" s="70" t="s">
+      <c r="H52" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I52" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3494,25 +3538,25 @@
         <v>82</v>
       </c>
       <c r="B53" s="6"/>
-      <c r="C53" s="7" t="s">
+      <c r="C53" s="112" t="s">
         <v>132</v>
       </c>
-      <c r="D53" s="75" t="s">
+      <c r="D53" s="74" t="s">
         <v>96</v>
       </c>
       <c r="E53" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F53" s="76" t="s">
+      <c r="F53" s="75" t="s">
         <v>97</v>
       </c>
-      <c r="G53" s="84" t="s">
+      <c r="G53" s="83" t="s">
         <v>76</v>
       </c>
-      <c r="H53" s="80" t="s">
-        <v>56</v>
-      </c>
-      <c r="I53" s="70" t="s">
+      <c r="H53" s="79" t="s">
+        <v>56</v>
+      </c>
+      <c r="I53" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3522,16 +3566,16 @@
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
-      <c r="F54" s="68" t="s">
+      <c r="F54" s="67" t="s">
         <v>60</v>
       </c>
       <c r="G54" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="H54" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I54" s="70" t="s">
+      <c r="H54" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I54" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3541,16 +3585,16 @@
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
-      <c r="F55" s="69" t="s">
+      <c r="F55" s="68" t="s">
         <v>45</v>
       </c>
       <c r="G55" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="H55" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I55" s="70" t="s">
+      <c r="H55" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I55" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3559,10 +3603,10 @@
         <v>83</v>
       </c>
       <c r="B56" s="6"/>
-      <c r="C56" s="6" t="s">
+      <c r="C56" s="114" t="s">
         <v>142</v>
       </c>
-      <c r="D56" s="75" t="s">
+      <c r="D56" s="74" t="s">
         <v>98</v>
       </c>
       <c r="E56" s="7" t="s">
@@ -3572,10 +3616,10 @@
         <v>100</v>
       </c>
       <c r="G56" s="22"/>
-      <c r="H56" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I56" s="70" t="s">
+      <c r="H56" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I56" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3585,16 +3629,16 @@
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
-      <c r="F57" s="68" t="s">
+      <c r="F57" s="67" t="s">
         <v>60</v>
       </c>
       <c r="G57" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="H57" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I57" s="70" t="s">
+      <c r="H57" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I57" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3604,16 +3648,16 @@
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
-      <c r="F58" s="69" t="s">
+      <c r="F58" s="68" t="s">
         <v>45</v>
       </c>
       <c r="G58" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="H58" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I58" s="70" t="s">
+      <c r="H58" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I58" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3622,10 +3666,10 @@
         <v>84</v>
       </c>
       <c r="B59" s="6"/>
-      <c r="C59" s="7" t="s">
+      <c r="C59" s="115" t="s">
         <v>131</v>
       </c>
-      <c r="D59" s="75" t="s">
+      <c r="D59" s="74" t="s">
         <v>99</v>
       </c>
       <c r="E59" s="7" t="s">
@@ -3634,13 +3678,13 @@
       <c r="F59" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="G59" s="74" t="s">
+      <c r="G59" s="73" t="s">
         <v>102</v>
       </c>
-      <c r="H59" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I59" s="70" t="s">
+      <c r="H59" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I59" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3650,16 +3694,16 @@
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
-      <c r="F60" s="68" t="s">
+      <c r="F60" s="67" t="s">
         <v>60</v>
       </c>
       <c r="G60" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="H60" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I60" s="70" t="s">
+      <c r="H60" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I60" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3669,16 +3713,16 @@
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
-      <c r="F61" s="69" t="s">
+      <c r="F61" s="68" t="s">
         <v>45</v>
       </c>
       <c r="G61" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="H61" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I61" s="70" t="s">
+      <c r="H61" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I61" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3687,10 +3731,10 @@
         <v>85</v>
       </c>
       <c r="B62" s="6"/>
-      <c r="C62" s="6" t="s">
+      <c r="C62" s="114" t="s">
         <v>130</v>
       </c>
-      <c r="D62" s="75" t="s">
+      <c r="D62" s="74" t="s">
         <v>103</v>
       </c>
       <c r="E62" s="7" t="s">
@@ -3699,13 +3743,13 @@
       <c r="F62" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="G62" s="74" t="s">
+      <c r="G62" s="73" t="s">
         <v>102</v>
       </c>
-      <c r="H62" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I62" s="70" t="s">
+      <c r="H62" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I62" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3715,16 +3759,16 @@
       <c r="C63" s="6"/>
       <c r="D63" s="6"/>
       <c r="E63" s="6"/>
-      <c r="F63" s="68" t="s">
+      <c r="F63" s="67" t="s">
         <v>60</v>
       </c>
       <c r="G63" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="H63" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I63" s="70" t="s">
+      <c r="H63" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I63" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3734,16 +3778,16 @@
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
       <c r="E64" s="4"/>
-      <c r="F64" s="69" t="s">
+      <c r="F64" s="68" t="s">
         <v>45</v>
       </c>
       <c r="G64" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="H64" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I64" s="70" t="s">
+      <c r="H64" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I64" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3752,10 +3796,10 @@
         <v>105</v>
       </c>
       <c r="B65" s="6"/>
-      <c r="C65" s="7" t="s">
+      <c r="C65" s="115" t="s">
         <v>129</v>
       </c>
-      <c r="D65" s="75" t="s">
+      <c r="D65" s="74" t="s">
         <v>124</v>
       </c>
       <c r="E65" s="7" t="s">
@@ -3764,13 +3808,13 @@
       <c r="F65" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="G65" s="74" t="s">
+      <c r="G65" s="73" t="s">
         <v>102</v>
       </c>
-      <c r="H65" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I65" s="70" t="s">
+      <c r="H65" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I65" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3780,16 +3824,16 @@
       <c r="C66" s="6"/>
       <c r="D66" s="6"/>
       <c r="E66" s="6"/>
-      <c r="F66" s="68" t="s">
+      <c r="F66" s="67" t="s">
         <v>60</v>
       </c>
       <c r="G66" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="H66" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I66" s="70" t="s">
+      <c r="H66" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I66" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3799,28 +3843,28 @@
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
-      <c r="F67" s="69" t="s">
+      <c r="F67" s="68" t="s">
         <v>45</v>
       </c>
       <c r="G67" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="H67" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I67" s="70" t="s">
+      <c r="H67" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I67" s="69" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="87" t="s">
+      <c r="A68" s="86" t="s">
         <v>143</v>
       </c>
       <c r="B68" s="60"/>
-      <c r="C68" s="61" t="s">
+      <c r="C68" s="116" t="s">
         <v>170</v>
       </c>
-      <c r="D68" s="75" t="s">
+      <c r="D68" s="74" t="s">
         <v>144</v>
       </c>
       <c r="E68" s="7" t="s">
@@ -3829,13 +3873,13 @@
       <c r="F68" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="G68" s="74" t="s">
+      <c r="G68" s="73" t="s">
         <v>102</v>
       </c>
-      <c r="H68" s="85" t="s">
+      <c r="H68" s="84" t="s">
         <v>92</v>
       </c>
-      <c r="I68" s="85" t="s">
+      <c r="I68" s="84" t="s">
         <v>61</v>
       </c>
     </row>
@@ -3843,91 +3887,91 @@
       <c r="A69" s="6"/>
       <c r="B69" s="6"/>
       <c r="C69" s="7"/>
-      <c r="D69" s="75"/>
+      <c r="D69" s="74"/>
       <c r="E69" s="7"/>
-      <c r="F69" s="68" t="s">
+      <c r="F69" s="67" t="s">
         <v>60</v>
       </c>
       <c r="G69" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="H69" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I69" s="70" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" s="86" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H69" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I69" s="69" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" s="85" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="6"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
       <c r="D70" s="6"/>
       <c r="E70" s="6"/>
-      <c r="F70" s="68" t="s">
+      <c r="F70" s="67" t="s">
         <v>45</v>
       </c>
       <c r="G70" s="61" t="s">
         <v>109</v>
       </c>
-      <c r="H70" s="105" t="s">
+      <c r="H70" s="102" t="s">
         <v>93</v>
       </c>
-      <c r="I70" s="98" t="s">
+      <c r="I70" s="95" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="71" spans="1:9" s="96" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="99" t="s">
+    <row r="71" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="96" t="s">
         <v>169</v>
       </c>
       <c r="B71" s="18"/>
-      <c r="C71" s="19" t="s">
+      <c r="C71" s="117" t="s">
         <v>171</v>
       </c>
-      <c r="D71" s="106" t="s">
+      <c r="D71" s="103" t="s">
         <v>168</v>
       </c>
       <c r="E71" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="F71" s="107" t="s">
+      <c r="F71" s="104" t="s">
         <v>166</v>
       </c>
-      <c r="G71" s="101" t="s">
+      <c r="G71" s="98" t="s">
         <v>102</v>
       </c>
-      <c r="H71" s="102" t="s">
+      <c r="H71" s="99" t="s">
         <v>92</v>
       </c>
-      <c r="I71" s="103" t="s">
+      <c r="I71" s="100" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="72" spans="1:9" s="96" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="24"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
-      <c r="D72" s="64" t="s">
+      <c r="D72" s="63" t="s">
         <v>165</v>
       </c>
       <c r="E72" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="F72" s="68" t="s">
+      <c r="F72" s="67" t="s">
         <v>60</v>
       </c>
       <c r="G72" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="H72" s="70" t="s">
+      <c r="H72" s="69" t="s">
         <v>56</v>
       </c>
       <c r="I72" s="28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="73" spans="1:9" s="96" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="36"/>
       <c r="B73" s="37"/>
       <c r="C73" s="37"/>
@@ -3935,28 +3979,28 @@
         <v>119</v>
       </c>
       <c r="E73" s="37"/>
-      <c r="F73" s="69" t="s">
+      <c r="F73" s="68" t="s">
         <v>45</v>
       </c>
       <c r="G73" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="H73" s="85" t="s">
+      <c r="H73" s="84" t="s">
         <v>92</v>
       </c>
-      <c r="I73" s="104" t="s">
+      <c r="I73" s="101" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="99" t="s">
+      <c r="A74" s="96" t="s">
         <v>113</v>
       </c>
       <c r="B74" s="18"/>
-      <c r="C74" s="19" t="s">
+      <c r="C74" s="117" t="s">
         <v>128</v>
       </c>
-      <c r="D74" s="100" t="s">
+      <c r="D74" s="97" t="s">
         <v>123</v>
       </c>
       <c r="E74" s="19" t="s">
@@ -3965,13 +4009,13 @@
       <c r="F74" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="G74" s="101" t="s">
+      <c r="G74" s="98" t="s">
         <v>102</v>
       </c>
-      <c r="H74" s="102" t="s">
+      <c r="H74" s="99" t="s">
         <v>92</v>
       </c>
-      <c r="I74" s="103" t="s">
+      <c r="I74" s="100" t="s">
         <v>61</v>
       </c>
     </row>
@@ -3981,13 +4025,13 @@
       <c r="C75" s="6"/>
       <c r="D75" s="6"/>
       <c r="E75" s="6"/>
-      <c r="F75" s="68" t="s">
+      <c r="F75" s="67" t="s">
         <v>60</v>
       </c>
       <c r="G75" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="H75" s="70" t="s">
+      <c r="H75" s="69" t="s">
         <v>56</v>
       </c>
       <c r="I75" s="28" t="s">
@@ -4000,16 +4044,16 @@
       <c r="C76" s="37"/>
       <c r="D76" s="37"/>
       <c r="E76" s="37"/>
-      <c r="F76" s="69" t="s">
+      <c r="F76" s="68" t="s">
         <v>45</v>
       </c>
       <c r="G76" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="H76" s="78" t="s">
+      <c r="H76" s="77" t="s">
         <v>93</v>
       </c>
-      <c r="I76" s="104" t="s">
+      <c r="I76" s="101" t="s">
         <v>61</v>
       </c>
     </row>
@@ -4018,10 +4062,10 @@
         <v>115</v>
       </c>
       <c r="B77" s="6"/>
-      <c r="C77" s="7" t="s">
+      <c r="C77" s="115" t="s">
         <v>174</v>
       </c>
-      <c r="D77" s="75" t="s">
+      <c r="D77" s="74" t="s">
         <v>116</v>
       </c>
       <c r="E77" s="7" t="s">
@@ -4030,13 +4074,13 @@
       <c r="F77" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="G77" s="84" t="s">
+      <c r="G77" s="83" t="s">
         <v>102</v>
       </c>
-      <c r="H77" s="80" t="s">
-        <v>56</v>
-      </c>
-      <c r="I77" s="80" t="s">
+      <c r="H77" s="79" t="s">
+        <v>56</v>
+      </c>
+      <c r="I77" s="79" t="s">
         <v>28</v>
       </c>
     </row>
@@ -4046,16 +4090,16 @@
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
       <c r="E78" s="6"/>
-      <c r="F78" s="68" t="s">
+      <c r="F78" s="67" t="s">
         <v>60</v>
       </c>
       <c r="G78" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="H78" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I78" s="70" t="s">
+      <c r="H78" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I78" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -4065,16 +4109,16 @@
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
       <c r="E79" s="4"/>
-      <c r="F79" s="69" t="s">
+      <c r="F79" s="68" t="s">
         <v>45</v>
       </c>
       <c r="G79" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="H79" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I79" s="70" t="s">
+      <c r="H79" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I79" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -4092,16 +4136,16 @@
       <c r="E80" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F80" s="79" t="s">
+      <c r="F80" s="78" t="s">
         <v>120</v>
       </c>
       <c r="G80" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="H80" s="80" t="s">
-        <v>56</v>
-      </c>
-      <c r="I80" s="80" t="s">
+      <c r="H80" s="79" t="s">
+        <v>56</v>
+      </c>
+      <c r="I80" s="79" t="s">
         <v>28</v>
       </c>
     </row>
@@ -4117,10 +4161,10 @@
       <c r="G81" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="H81" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I81" s="70" t="s">
+      <c r="H81" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I81" s="69" t="s">
         <v>28</v>
       </c>
     </row>
@@ -4130,31 +4174,31 @@
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
       <c r="E82" s="4"/>
-      <c r="F82" s="69" t="s">
+      <c r="F82" s="68" t="s">
         <v>45</v>
       </c>
       <c r="G82" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="H82" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I82" s="70" t="s">
+      <c r="H82" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I82" s="69" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="87" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="81" t="s">
+      <c r="A83" s="80" t="s">
         <v>125</v>
       </c>
-      <c r="B83" s="81"/>
-      <c r="C83" s="97" t="s">
+      <c r="B83" s="80"/>
+      <c r="C83" s="94" t="s">
         <v>172</v>
       </c>
       <c r="D83" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="E83" s="82" t="s">
+      <c r="E83" s="81" t="s">
         <v>58</v>
       </c>
       <c r="F83" s="20" t="s">
@@ -4163,48 +4207,48 @@
       <c r="G83" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="H83" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I83" s="70" t="s">
+      <c r="H83" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I83" s="69" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="81"/>
-      <c r="B84" s="81"/>
-      <c r="C84" s="81"/>
-      <c r="D84" s="81"/>
-      <c r="E84" s="81"/>
+      <c r="A84" s="80"/>
+      <c r="B84" s="80"/>
+      <c r="C84" s="80"/>
+      <c r="D84" s="80"/>
+      <c r="E84" s="80"/>
       <c r="F84" s="11" t="s">
         <v>126</v>
       </c>
       <c r="G84" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="H84" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I84" s="70" t="s">
+      <c r="H84" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I84" s="69" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="83"/>
-      <c r="B85" s="83"/>
-      <c r="C85" s="83"/>
-      <c r="D85" s="83"/>
-      <c r="E85" s="83"/>
-      <c r="F85" s="69" t="s">
+      <c r="A85" s="82"/>
+      <c r="B85" s="82"/>
+      <c r="C85" s="82"/>
+      <c r="D85" s="82"/>
+      <c r="E85" s="82"/>
+      <c r="F85" s="68" t="s">
         <v>45</v>
       </c>
       <c r="G85" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="H85" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I85" s="70" t="s">
+      <c r="H85" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I85" s="69" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>